<commit_message>
Add AI wrapper risk analysis and update recommendations
- New sheet: Риски AI-обёрток (wrapper graveyard, survival stats, what works vs dies)
- Updated Идеи для тебя: split into SAFE / RISKY / AVOID categories
- Added concrete failure examples: Jasper (-54%), Builder.ai (bankrupt), Phind (dead after $10M raise)
- Key insight: AI as component inside product survives, AI as product dies

Made-with: Cursor
</commit_message>
<xml_diff>
--- a/yc_startups_analysis.xlsx
+++ b/yc_startups_analysis.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Топ для соло" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Аналитика" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Идеи для тебя" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Риски AI-обёрток" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -20,7 +21,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -33,8 +34,13 @@
       <color rgb="00FFFFFF"/>
       <sz val="11"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -53,6 +59,18 @@
         <bgColor rgb="FF1E7145"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8B0000"/>
+        <bgColor rgb="FF8B0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB8860B"/>
+        <bgColor rgb="FFB8860B"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -66,7 +84,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -77,6 +95,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -5438,7 +5461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5979,83 +6002,372 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="inlineStr">
-        <is>
-          <t>WINNER IDEAS (easiest to start, highest signal):</t>
-        </is>
-      </c>
-      <c r="B13" s="3" t="n"/>
-      <c r="C13" s="3" t="n"/>
-      <c r="D13" s="3" t="n"/>
-      <c r="E13" s="3" t="n"/>
-      <c r="F13" s="3" t="n"/>
-      <c r="G13" s="3" t="n"/>
-      <c r="H13" s="3" t="n"/>
-      <c r="I13" s="3" t="n"/>
-      <c r="J13" s="3" t="n"/>
+      <c r="A13" s="3" t="inlineStr"/>
+      <c r="B13" s="3" t="inlineStr"/>
+      <c r="C13" s="3" t="inlineStr"/>
+      <c r="D13" s="3" t="inlineStr"/>
+      <c r="E13" s="3" t="inlineStr"/>
+      <c r="F13" s="3" t="inlineStr"/>
+      <c r="G13" s="3" t="inlineStr"/>
+      <c r="H13" s="3" t="inlineStr"/>
+      <c r="I13" s="3" t="inlineStr"/>
+      <c r="J13" s="3" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="inlineStr">
-        <is>
-          <t>#1 BEST START</t>
-        </is>
-      </c>
-      <c r="B14" s="3" t="inlineStr">
-        <is>
-          <t>AI copilot for specific profession</t>
-        </is>
-      </c>
-      <c r="C14" s="3" t="inlineStr">
-        <is>
-          <t>Low competition in niches, recurring SaaS, no infra headaches, build in 3-4 weeks</t>
-        </is>
-      </c>
-      <c r="D14" s="3" t="n"/>
-      <c r="E14" s="3" t="n"/>
-      <c r="F14" s="3" t="n"/>
-      <c r="G14" s="3" t="n"/>
-      <c r="H14" s="3" t="n"/>
-      <c r="I14" s="3" t="n"/>
+      <c r="A14" s="3">
+        <f>== ПЕРЕСМОТРЕННЫЕ РЕКОМЕНДАЦИИ (с учётом рисков AI-обёрток) ===</f>
+        <v/>
+      </c>
+      <c r="B14" s="3" t="inlineStr"/>
+      <c r="C14" s="3" t="inlineStr"/>
+      <c r="D14" s="3" t="inlineStr"/>
+      <c r="E14" s="3" t="inlineStr"/>
+      <c r="F14" s="3" t="inlineStr"/>
+      <c r="G14" s="3" t="inlineStr"/>
+      <c r="H14" s="3" t="inlineStr"/>
+      <c r="I14" s="3" t="inlineStr"/>
       <c r="J14" s="3" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="inlineStr">
-        <is>
-          <t>#2 BEST START</t>
-        </is>
-      </c>
-      <c r="B15" s="3" t="inlineStr">
-        <is>
-          <t>Voice AI agent for local service business</t>
-        </is>
-      </c>
-      <c r="C15" s="3" t="inlineStr">
-        <is>
-          <t>Vapi API handles complexity, local businesses pay well, easy to sell via cold outreach</t>
-        </is>
-      </c>
-      <c r="D15" s="3" t="n"/>
-      <c r="E15" s="3" t="n"/>
-      <c r="F15" s="3" t="n"/>
-      <c r="G15" s="3" t="n"/>
-      <c r="H15" s="3" t="n"/>
-      <c r="I15" s="3" t="n"/>
-      <c r="J15" s="3" t="n"/>
+      <c r="A15" s="3" t="inlineStr"/>
+      <c r="B15" s="3" t="inlineStr"/>
+      <c r="C15" s="3" t="inlineStr"/>
+      <c r="D15" s="3" t="inlineStr"/>
+      <c r="E15" s="3" t="inlineStr"/>
+      <c r="F15" s="3" t="inlineStr"/>
+      <c r="G15" s="3" t="inlineStr"/>
+      <c r="H15" s="3" t="inlineStr"/>
+      <c r="I15" s="3" t="inlineStr"/>
+      <c r="J15" s="3" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>#3 BEST START</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Browser automation product for specific workflow</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Browser Use handles infra, just build the UX and business logic on top</t>
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>SAFE: Не обёртки, OpenAI не конкурент</t>
+        </is>
+      </c>
+      <c r="B16" s="6" t="inlineStr"/>
+      <c r="C16" s="6" t="inlineStr"/>
+      <c r="D16" s="6" t="inlineStr"/>
+      <c r="E16" s="6" t="inlineStr"/>
+      <c r="F16" s="6" t="inlineStr"/>
+      <c r="G16" s="6" t="inlineStr"/>
+      <c r="H16" s="6" t="inlineStr"/>
+      <c r="I16" s="6" t="inlineStr"/>
+      <c r="J16" s="6" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>#1</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Open-source dev tool (auth/UI/infra)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Better Auth, assistant-ui, NextUI</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Community moat, OpenAI не делает OSS библиотеки</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>TypeScript</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>OSS + Hosted SaaS</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>2</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>4-6 нед.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>#2</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Нишевый SaaS где AI = фича (не продукт)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Tremor, Laminar</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>CRM для фотографов, дашборд для строителей — AI внутри, но не основа</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>React + DB + API</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>SaaS $49-199/mo</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>3</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>6-8 нед.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>#3</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Микро-утилита а ля FormulaBot</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>FormulaBot ($500K, 87% margin)</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Узкая задача, мизерные token costs, SEO-дистрибуция</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Next.js + LLM</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Freemium SaaS</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>2-4 нед.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>RISKY: AI-обёртки, но с возможной защитой через нишу/дистрибуцию</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="7" t="inlineStr">
+        <is>
+          <t>#4</t>
+        </is>
+      </c>
+      <c r="B22" s="7" t="inlineStr">
+        <is>
+          <t>AI-тренажёр переговоров/интервью</t>
+        </is>
+      </c>
+      <c r="C22" s="7" t="inlineStr">
+        <is>
+          <t>Solidroad</t>
+        </is>
+      </c>
+      <c r="D22" s="7" t="inlineStr">
+        <is>
+          <t>Нишевый контент + дистрибуция защищает, но ChatGPT Voice давит</t>
+        </is>
+      </c>
+      <c r="E22" s="7" t="inlineStr">
+        <is>
+          <t>React + Voice API</t>
+        </is>
+      </c>
+      <c r="F22" s="7" t="inlineStr">
+        <is>
+          <t>SaaS $19-49/mo</t>
+        </is>
+      </c>
+      <c r="G22" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="H22" s="7" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I22" s="7" t="inlineStr">
+        <is>
+          <t>3-5 нед.</t>
+        </is>
+      </c>
+      <c r="J22" s="7" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>#5</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>AI-copilot для 1 профессии (узкая)</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Cactus, MagicSchool</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Работает ЕСЛИ AI не главное — а workflow + интеграции + данные</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Next.js + LLM API</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>SaaS $29-79/mo</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>2</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Medium-High</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>3-4 нед.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>AVOID: Высокий риск смерти от платформ</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="B26" s="8" t="inlineStr">
+        <is>
+          <t>Voice AI агент</t>
+        </is>
+      </c>
+      <c r="C26" s="8" t="inlineStr">
+        <is>
+          <t>Vapi сам сделает UI, OpenAI Realtime API дешевеет</t>
+        </is>
+      </c>
+      <c r="D26" s="8" t="n"/>
+      <c r="E26" s="8" t="n"/>
+      <c r="F26" s="8" t="n"/>
+      <c r="G26" s="8" t="n"/>
+      <c r="H26" s="8" t="n"/>
+      <c r="I26" s="8" t="n"/>
+      <c r="J26" s="8" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>AI research assistant</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ChatGPT Deep Research + Claude уже делают это</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Browser automation product</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>OpenAI Operator + Google уже здесь</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>AI document parser (PDF/docs)</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>ChatGPT/Claude читают PDF нативно, категория мертва</t>
         </is>
       </c>
     </row>
@@ -6065,4 +6377,741 @@
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4">
+        <f>== КЛАДБИЩЕ AI-ОБЁРТОК: КОНКРЕТНЫЕ ПРИМЕРЫ ===</f>
+        <v/>
+      </c>
+      <c r="B1" s="4" t="n"/>
+      <c r="C1" s="4" t="n"/>
+      <c r="D1" s="4" t="n"/>
+      <c r="E1" s="4" t="n"/>
+      <c r="F1" s="4" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>Стартап</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>Funding</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>Оценка</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>Что случилось</t>
+        </is>
+      </c>
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t>Причина смерти</t>
+        </is>
+      </c>
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t>Источник</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Jasper AI</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>$131M</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>$1.5B</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Revenue упал с $120M до $55M (-54%), CEO уволен, оценка -20%</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>ChatGPT дал бесплатно то за что Jasper брал $80/мес</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Latka, Maginative</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Builder.ai</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>$445M</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>$1.2B</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Банкрот (май 2025). Реальный revenue $55M при заявленном $220M</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Не было реального AI — 1500 человек в Индии/Украине</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Bloomberg, TechStartups</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Phind</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>$10M Series A</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Закрылся через месяц после раунда (январь 2026)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ChatGPT/Claude/Google добавили нативный поиск</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>IntelligentTools</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CodeParrot (YC W23)</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>$500K</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Пик MRR = $1,500. Закрылся июль 2025</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Cursor/Claude делают Figma-to-code нативно</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Entrepreneur</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Chat with PDF (десятки)</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>разный</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Все умерли в один день (октябрь 2023)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>ChatGPT добавил загрузку PDF бесплатно</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Gizmodo, TechCrunch</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <f>== СТАТИСТИКА ВЫЖИВАЕМОСТИ AI-ОБЁРТОК ===</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Метрика</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Значение</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Источник</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Процент полных провалов</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>80-95%</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>RAND Corporation, MIT 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Доходят до $10K/мес revenue</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2-5%</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Market Clarity</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Новые обёртки запускаются каждый день</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>10-15 штук</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Market Clarity</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Стартапов закрылось в USA (2024)</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>966 (+25.6% к 2023)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>SimpleClosure</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>AI-инструментов закрылись (2025)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>227</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>SimpleClosure</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>YC AI-стартапов — обёртки с низкой ценностью</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>41%</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Stanford Research</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Gross margin AI-обёртки</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>25-60%</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Bessemer VP 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Gross margin обычного SaaS</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>70-80%</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Bessemer VP 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Время копирования фичи конкурентом</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>3-6 месяцев</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Virta Ventures</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>LLM API цены упали за 16 месяцев</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>-83%</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>OpenAI / FutureSearch</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Годовой churn customer support AI</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>76%</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>LiveX AI</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>OpenAI потери при $3.7B revenue (2024)</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>$5B</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Medium/PYMNTS</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <f>== КТО ВЫЖИЛ И ПОЧЕМУ ===</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Стартап</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Оценка</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Почему жив (moat)</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Модель</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Ключевой урок</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Harvey AI</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>$75M ARR</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>$5B</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Проприетарные юридические модели + комплаенс + workflow</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Deep vertical (Legal)</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>OpenAI не будет продавать в каждую юрфирму</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Copy.ai</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>$23.7M ARR</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Быстро стал workflow-платформой для GTM-команд, не обёрткой</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Pivot из обёртки в платформу</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Выжил с $17M vs Jasper с $131M</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>FormulaBot</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>$500K ARR, 87.5% margin</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Узкая ниша (текст→Excel формулы), мизерные token costs</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Микро-утилита с SEO</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Маленький рынок = безопасность от больших</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Perplexity</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>$100M ARR</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>$20B</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Свой поисковый индекс + citation system + open-source модели</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Инфраструктура &gt; обёртка</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Стал не обёрткой а платформой</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>PDF.ai</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>400K users</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>100x дистрибуция конкурента с лучшим AI</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Дистрибуция &gt; технология</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>SEO + бренд важнее качества AI</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <f>== ПАТТЕРН: ЧТО УМИРАЕТ vs ЧТО ВЫЖИВАЕТ ===</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>УМИРАЕТ</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>ВЫЖИВАЕТ</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Мы делаем X, но с AI</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Мы решаем проблему Y в индустрии Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>UI поверх API</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Workflow + данные + интеграции + комплаенс</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Горизонтальный продукт</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Глубокая вертикаль</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Конкурирует с ChatGPT</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Конкурирует с легаси-софтом (Excel, SAP, 1С)</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Технология = продукт</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Дистрибуция = продукт</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>AI — единственная ценность</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>AI — один из компонентов бизнес-продукта</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add comprehensive AI Infrastructure ideas analysis sheet
New sheet "AI Infra идеи" with:
- 10 detailed startup ideas (MCP tooling, agent observability, security, DX)
- Full breakdown: pain point, competitors, open-core model, tech stack, MVP timeline
- Market context with key metrics (MCP SDK 97M downloads, 79% build failures)
- Ranked recommendations with scores and rationale
- Launch strategies (quick/balanced/ambitious/combo)
- AI wrappers vs AI infra comparison table
- Bar chart (idea ratings) and pie chart (category distribution)

Made-with: Cursor
</commit_message>
<xml_diff>
--- a/yc_startups_analysis.xlsx
+++ b/yc_startups_analysis.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Аналитика" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Идеи для тебя" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Риски AI-обёрток" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="AI Infra идеи" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -21,7 +22,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -39,8 +40,26 @@
       <color rgb="00FFFFFF"/>
       <sz val="12"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="FF1A1A2E"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
+    <font/>
+    <font>
+      <b val="1"/>
+      <color rgb="FF1A1A2E"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="17">
     <fill>
       <patternFill/>
     </fill>
@@ -71,6 +90,72 @@
         <bgColor rgb="FFB8860B"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F5E9"/>
+        <bgColor rgb="FFE8F5E9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2E7D32"/>
+        <bgColor rgb="FF2E7D32"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE3F2FD"/>
+        <bgColor rgb="FFE3F2FD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1565C0"/>
+        <bgColor rgb="FF1565C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF3E0"/>
+        <bgColor rgb="00FFF3E0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE65100"/>
+        <bgColor rgb="FFE65100"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC8E6C9"/>
+        <bgColor rgb="FFC8E6C9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF8E1"/>
+        <bgColor rgb="00FFF8E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF57F17"/>
+        <bgColor rgb="FFF57F17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE4EC"/>
+        <bgColor rgb="FFFCE4EC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC62828"/>
+        <bgColor rgb="FFC62828"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -84,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -100,6 +185,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -529,6 +630,191 @@
 </chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>AI Infra \u0438\u0434\u0435\u0438: \u0440\u0435\u0439\u0442\u0438\u043d\u0433 \u0434\u043b\u044f \u0441\u043e\u043b\u043e-\u0440\u0430\u0437\u0440\u0430\u0431\u043e\u0442\u0447\u0438\u043a\u0430</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'AI Infra идеи'!G28</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'AI Infra идеи'!$F$29:$F$38</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'AI Infra идеи'!$G$29:$G$38</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="1"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>\u0418\u0434\u0435\u044f</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Score (1-10)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>\u0420\u0430\u0441\u043f\u0440\u0435\u0434\u0435\u043b\u0435\u043d\u0438\u0435 \u0438\u0434\u0435\u0439 \u043f\u043e \u043a\u0430\u0442\u0435\u0433\u043e\u0440\u0438\u044f\u043c</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'AI Infra идеи'!J28</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'AI Infra идеи'!$I$29:$I$34</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'AI Infra идеи'!$J$29:$J$34</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="1"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
@@ -600,6 +886,55 @@
 </wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="YC_Startups" displayName="YC_Startups" ref="A1:Q41" headerRowCount="1">
   <autoFilter ref="A1:Q41"/>
@@ -663,6 +998,30 @@
     <tableColumn id="10" name="Risk"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="AIInfraIdeas" displayName="AIInfraIdeas" ref="A3:O13" headerRowCount="1">
+  <autoFilter ref="A3:O13"/>
+  <tableColumns count="15">
+    <tableColumn id="1" name="#"/>
+    <tableColumn id="2" name="Идея"/>
+    <tableColumn id="3" name="Категория"/>
+    <tableColumn id="4" name="Боль которую решает"/>
+    <tableColumn id="5" name="Конкуренты"/>
+    <tableColumn id="6" name="Почему конкуренты слабые"/>
+    <tableColumn id="7" name="Open Core: Free"/>
+    <tableColumn id="8" name="Open Core: Paid"/>
+    <tableColumn id="9" name="Стек"/>
+    <tableColumn id="10" name="MVP (недели)"/>
+    <tableColumn id="11" name="Сложность (1-5)"/>
+    <tableColumn id="12" name="Revenue потенциал"/>
+    <tableColumn id="13" name="AI-wrapper риск"/>
+    <tableColumn id="14" name="Первые клиенты"/>
+    <tableColumn id="15" name="Путь к $10K MRR"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -7114,4 +7473,1685 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9">
+        <f>== AI INFRASTRUCTURE ИДЕИ: ПОЛНЫЙ АНАЛИЗ ===</f>
+        <v/>
+      </c>
+      <c r="B1" s="9" t="n"/>
+      <c r="C1" s="9" t="n"/>
+      <c r="D1" s="9" t="n"/>
+      <c r="E1" s="9" t="n"/>
+      <c r="F1" s="9" t="n"/>
+      <c r="G1" s="9" t="n"/>
+      <c r="H1" s="9" t="n"/>
+      <c r="I1" s="9" t="n"/>
+      <c r="J1" s="9" t="n"/>
+      <c r="K1" s="9" t="n"/>
+      <c r="L1" s="9" t="n"/>
+      <c r="M1" s="9" t="n"/>
+      <c r="N1" s="9" t="n"/>
+      <c r="O1" s="9" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="10" t="inlineStr">
+        <is>
+          <t>#</t>
+        </is>
+      </c>
+      <c r="B3" s="10" t="inlineStr">
+        <is>
+          <t>Идея</t>
+        </is>
+      </c>
+      <c r="C3" s="10" t="inlineStr">
+        <is>
+          <t>Категория</t>
+        </is>
+      </c>
+      <c r="D3" s="10" t="inlineStr">
+        <is>
+          <t>Боль которую решает</t>
+        </is>
+      </c>
+      <c r="E3" s="10" t="inlineStr">
+        <is>
+          <t>Конкуренты</t>
+        </is>
+      </c>
+      <c r="F3" s="10" t="inlineStr">
+        <is>
+          <t>Почему конкуренты слабые</t>
+        </is>
+      </c>
+      <c r="G3" s="10" t="inlineStr">
+        <is>
+          <t>Open Core: Free</t>
+        </is>
+      </c>
+      <c r="H3" s="10" t="inlineStr">
+        <is>
+          <t>Open Core: Paid</t>
+        </is>
+      </c>
+      <c r="I3" s="10" t="inlineStr">
+        <is>
+          <t>Стек</t>
+        </is>
+      </c>
+      <c r="J3" s="10" t="inlineStr">
+        <is>
+          <t>MVP (недели)</t>
+        </is>
+      </c>
+      <c r="K3" s="10" t="inlineStr">
+        <is>
+          <t>Сложность (1-5)</t>
+        </is>
+      </c>
+      <c r="L3" s="10" t="inlineStr">
+        <is>
+          <t>Revenue потенциал</t>
+        </is>
+      </c>
+      <c r="M3" s="10" t="inlineStr">
+        <is>
+          <t>AI-wrapper риск</t>
+        </is>
+      </c>
+      <c r="N3" s="10" t="inlineStr">
+        <is>
+          <t>Первые клиенты</t>
+        </is>
+      </c>
+      <c r="O3" s="10" t="inlineStr">
+        <is>
+          <t>Путь к $10K MRR</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="inlineStr">
+        <is>
+          <t>MCP Test Framework</t>
+        </is>
+      </c>
+      <c r="C4" s="11" t="inlineStr">
+        <is>
+          <t>MCP Tooling</t>
+        </is>
+      </c>
+      <c r="D4" s="11" t="inlineStr">
+        <is>
+          <t>79% MCP-серверов не собираются, нет стандартного способа протестировать MCP-сервер до деплоя. Нет CI/CD для MCP.</t>
+        </is>
+      </c>
+      <c r="E4" s="11" t="inlineStr">
+        <is>
+          <t>MCP Inspector (официальный, ручной debug)</t>
+        </is>
+      </c>
+      <c r="F4" s="11" t="inlineStr">
+        <is>
+          <t>Только ручной дебаг. Нет автотестов, нет CI/CD, нет регрессии. Никто не делает полноценный тест-фреймворк.</t>
+        </is>
+      </c>
+      <c r="G4" s="11" t="inlineStr">
+        <is>
+          <t>CLI тест-раннер: запуск, проверка list_tools, валидация схем, снэпшоты</t>
+        </is>
+      </c>
+      <c r="H4" s="11" t="inlineStr">
+        <is>
+          <t>CI/CD GitHub Action, badge 'MCP Verified', hosted dashboard с историей тестов, уведомления о поломках</t>
+        </is>
+      </c>
+      <c r="I4" s="11" t="inlineStr">
+        <is>
+          <t>TypeScript, Node.js, MCP SDK</t>
+        </is>
+      </c>
+      <c r="J4" s="11" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+      <c r="K4" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" s="11" t="inlineStr">
+        <is>
+          <t>Средний</t>
+        </is>
+      </c>
+      <c r="M4" s="11" t="inlineStr">
+        <is>
+          <t>Нулевой</t>
+        </is>
+      </c>
+      <c r="N4" s="11" t="inlineStr">
+        <is>
+          <t>MCP-разработчики, авторы серверов из реестра, open-source комьюнити</t>
+        </is>
+      </c>
+      <c r="O4" s="11" t="inlineStr">
+        <is>
+          <t>GitHub Action подписка $29/мес на команду. 350 команд = $10K MRR. При 10K+ MCP-серверов — реально.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="11" t="inlineStr">
+        <is>
+          <t>AI Agent Cost Tracker</t>
+        </is>
+      </c>
+      <c r="C5" s="11" t="inlineStr">
+        <is>
+          <t>Agent Observability</t>
+        </is>
+      </c>
+      <c r="D5" s="11" t="inlineStr">
+        <is>
+          <t>Разработчики и команды не знают сколько тратят на LLM API. Случаи $800K счетов при $250K revenue. Нет бюджетирования.</t>
+        </is>
+      </c>
+      <c r="E5" s="11" t="inlineStr">
+        <is>
+          <t>AgentReplay (observability, не billing), Helicone (closed-source), OpenLit (широкий)</t>
+        </is>
+      </c>
+      <c r="F5" s="11" t="inlineStr">
+        <is>
+          <t>Никто не фокусируется на COST/BUDGET. Все делают traces/observability. Лёгкого OSS budget-трекера нет.</t>
+        </is>
+      </c>
+      <c r="G5" s="11" t="inlineStr">
+        <is>
+          <t>Локальный прокси/SDK: перехват LLM-вызовов, подсчёт токенов/$, дашборд, алерты</t>
+        </is>
+      </c>
+      <c r="H5" s="11" t="inlineStr">
+        <is>
+          <t>Team dashboard, бюджеты по проектам, billing integration (Stripe), алерты Slack/email, отчёты</t>
+        </is>
+      </c>
+      <c r="I5" s="11" t="inlineStr">
+        <is>
+          <t>TypeScript/Python, Proxy, SQLite/Postgres, React dashboard</t>
+        </is>
+      </c>
+      <c r="J5" s="11" t="inlineStr">
+        <is>
+          <t>2-3</t>
+        </is>
+      </c>
+      <c r="K5" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="11" t="inlineStr">
+        <is>
+          <t>Средний-высокий</t>
+        </is>
+      </c>
+      <c r="M5" s="11" t="inlineStr">
+        <is>
+          <t>Нулевой</t>
+        </is>
+      </c>
+      <c r="N5" s="11" t="inlineStr">
+        <is>
+          <t>AI-стартапы, фрилансеры, команды с LLM API в продакшене. Twitter/HN launch.</t>
+        </is>
+      </c>
+      <c r="O5" s="11" t="inlineStr">
+        <is>
+          <t>$19/мес на команду. 530 команд = $10K. Боль у всех — распространение через OSS быстрое.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="11" t="inlineStr">
+        <is>
+          <t>MCP Package Manager</t>
+        </is>
+      </c>
+      <c r="C6" s="11" t="inlineStr">
+        <is>
+          <t>MCP Tooling</t>
+        </is>
+      </c>
+      <c r="D6" s="11" t="inlineStr">
+        <is>
+          <t>Найти и установить MCP-сервер = 'византийский процесс'. Нет npm install для MCP. Ручная настройка каждого.</t>
+        </is>
+      </c>
+      <c r="E6" s="11" t="inlineStr">
+        <is>
+          <t>Офиц. реестр (зачаточный), mcp.run (hosted, не OSS), Smithery</t>
+        </is>
+      </c>
+      <c r="F6" s="11" t="inlineStr">
+        <is>
+          <t>Офиц. реестр — только каталог, не package manager. mcp.run — closed. Нет `mcp install X` как npm.</t>
+        </is>
+      </c>
+      <c r="G6" s="11" t="inlineStr">
+        <is>
+          <t>CLI: `mcp install stripe`, `mcp search`, `mcp update`. Авто-конфиг для Cursor/Claude. Public registry.</t>
+        </is>
+      </c>
+      <c r="H6" s="11" t="inlineStr">
+        <is>
+          <t>Private registry для компаний, team management, security scanning серверов, аналитика использования</t>
+        </is>
+      </c>
+      <c r="I6" s="11" t="inlineStr">
+        <is>
+          <t>TypeScript, Node.js, SQLite/Postgres, CLI (Commander/Clack)</t>
+        </is>
+      </c>
+      <c r="J6" s="11" t="inlineStr">
+        <is>
+          <t>6-8</t>
+        </is>
+      </c>
+      <c r="K6" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="L6" s="11" t="inlineStr">
+        <is>
+          <t>Очень высокий</t>
+        </is>
+      </c>
+      <c r="M6" s="11" t="inlineStr">
+        <is>
+          <t>Нулевой</t>
+        </is>
+      </c>
+      <c r="N6" s="11" t="inlineStr">
+        <is>
+          <t>Все кто использует MCP: Cursor-юзеры, Claude Code, компании с AI-агентами</t>
+        </is>
+      </c>
+      <c r="O6" s="11" t="inlineStr">
+        <is>
+          <t>Private registry $49/мес. 200 компаний = $10K. Если станет стандартом — как npm ($100M+ revenue).</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="11" t="inlineStr">
+        <is>
+          <t>MCP Auth &amp; Security Middleware</t>
+        </is>
+      </c>
+      <c r="C7" s="11" t="inlineStr">
+        <is>
+          <t>MCP Security</t>
+        </is>
+      </c>
+      <c r="D7" s="11" t="inlineStr">
+        <is>
+          <t>MCP-сервера = дыра в безопасности. Нет стандартной auth. Токены текут. Enterprise боятся внедрять.</t>
+        </is>
+      </c>
+      <c r="E7" s="11" t="inlineStr">
+        <is>
+          <t>Kong MCP Gateway (enterprise, дорого), Azure APIM (завязан на Azure), Red Hat (гайды)</t>
+        </is>
+      </c>
+      <c r="F7" s="11" t="inlineStr">
+        <is>
+          <t>Все конкуренты — enterprise/vendor-locked. Лёгкого OSS прокси который поставил и работает — нет.</t>
+        </is>
+      </c>
+      <c r="G7" s="11" t="inlineStr">
+        <is>
+          <t>Прокси между агентом и MCP: auth (API key/OAuth), фильтрация tool calls, логи</t>
+        </is>
+      </c>
+      <c r="H7" s="11" t="inlineStr">
+        <is>
+          <t>SSO (Okta/Azure AD), audit trail, комплаенс-отчёты, role-based tool access, hosted proxy, PII фильтрация</t>
+        </is>
+      </c>
+      <c r="I7" s="11" t="inlineStr">
+        <is>
+          <t>TypeScript/Go, HTTP proxy, OAuth2, SQLite/Postgres</t>
+        </is>
+      </c>
+      <c r="J7" s="11" t="inlineStr">
+        <is>
+          <t>4-6</t>
+        </is>
+      </c>
+      <c r="K7" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="L7" s="11" t="inlineStr">
+        <is>
+          <t>Высокий</t>
+        </is>
+      </c>
+      <c r="M7" s="11" t="inlineStr">
+        <is>
+          <t>Нулевой</t>
+        </is>
+      </c>
+      <c r="N7" s="11" t="inlineStr">
+        <is>
+          <t>Enterprise компании с compliance требованиями (SOC2, HIPAA). Стартапы с AI-агентами.</t>
+        </is>
+      </c>
+      <c r="O7" s="11" t="inlineStr">
+        <is>
+          <t>Enterprise plan $199/мес. 50 компаний = $10K. Enterprise платят много за security.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="11" t="inlineStr">
+        <is>
+          <t>OpenAPI ↔ MCP конвертер</t>
+        </is>
+      </c>
+      <c r="C8" s="11" t="inlineStr">
+        <is>
+          <t>MCP Tooling</t>
+        </is>
+      </c>
+      <c r="D8" s="11" t="inlineStr">
+        <is>
+          <t>У компаний тысячи REST API с OpenAPI spec. Чтобы AI-агент их вызывал через MCP — каждый сервер пишут руками.</t>
+        </is>
+      </c>
+      <c r="E8" s="11" t="inlineStr">
+        <is>
+          <t>Единичные скрипты на GitHub, ничего production-ready</t>
+        </is>
+      </c>
+      <c r="F8" s="11" t="inlineStr">
+        <is>
+          <t>Скрипты не поддерживают auth, pagination, webhooks, error handling. Нет auto-sync.</t>
+        </is>
+      </c>
+      <c r="G8" s="11" t="inlineStr">
+        <is>
+          <t>CLI: скормил openapi.yaml → получил MCP-сервер. Обратно: MCP → OpenAPI spec.</t>
+        </is>
+      </c>
+      <c r="H8" s="11" t="inlineStr">
+        <is>
+          <t>Hosted конвертер с auto-sync (обновился API → обновился MCP), кастомные правила, мониторинг</t>
+        </is>
+      </c>
+      <c r="I8" s="11" t="inlineStr">
+        <is>
+          <t>TypeScript, Node.js, OpenAPI Parser, MCP SDK</t>
+        </is>
+      </c>
+      <c r="J8" s="11" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+      <c r="K8" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="L8" s="11" t="inlineStr">
+        <is>
+          <t>Высокий</t>
+        </is>
+      </c>
+      <c r="M8" s="11" t="inlineStr">
+        <is>
+          <t>Нулевой</t>
+        </is>
+      </c>
+      <c r="N8" s="11" t="inlineStr">
+        <is>
+          <t>Любая компания с REST API которая хочет поддержку AI-агентов. SaaS-компании.</t>
+        </is>
+      </c>
+      <c r="O8" s="11" t="inlineStr">
+        <is>
+          <t>Auto-sync $39/мес на API. 260 API = $10K. Каждый SaaS захочет MCP для своего API.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="11" t="inlineStr">
+        <is>
+          <t>Unified Agent Config Manager</t>
+        </is>
+      </c>
+      <c r="C9" s="11" t="inlineStr">
+        <is>
+          <t>Agent DX</t>
+        </is>
+      </c>
+      <c r="D9" s="11" t="inlineStr">
+        <is>
+          <t>Каждый AI-агент имеет свой формат: .cursor/rules, CLAUDE.md, AGENTS.md, copilot-instructions.md. Пишешь одно и то же 4 раза.</t>
+        </is>
+      </c>
+      <c r="E9" s="11" t="inlineStr">
+        <is>
+          <t>RuleBox.ai (ручной агрегатор)</t>
+        </is>
+      </c>
+      <c r="F9" s="11" t="inlineStr">
+        <is>
+          <t>RuleBox — просто каталог готовых rules. Нет автосинхронизации, нет CLI, нет конвертации.</t>
+        </is>
+      </c>
+      <c r="G9" s="11" t="inlineStr">
+        <is>
+          <t>CLI: один конфиг agent.yaml → генерация для всех агентов. `agent-config sync`</t>
+        </is>
+      </c>
+      <c r="H9" s="11" t="inlineStr">
+        <is>
+          <t>Team sync через cloud, CI/CD hook (обновил код → обновились rules), аналитика, team dashboard</t>
+        </is>
+      </c>
+      <c r="I9" s="11" t="inlineStr">
+        <is>
+          <t>TypeScript, Node.js, YAML parser, CLI (Commander/Clack)</t>
+        </is>
+      </c>
+      <c r="J9" s="11" t="inlineStr">
+        <is>
+          <t>2-3</t>
+        </is>
+      </c>
+      <c r="K9" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="11" t="inlineStr">
+        <is>
+          <t>Средний</t>
+        </is>
+      </c>
+      <c r="M9" s="11" t="inlineStr">
+        <is>
+          <t>Нулевой</t>
+        </is>
+      </c>
+      <c r="N9" s="11" t="inlineStr">
+        <is>
+          <t>Разработчики использующие 2+ AI-агентов одновременно (Cursor + Claude + Copilot)</t>
+        </is>
+      </c>
+      <c r="O9" s="11" t="inlineStr">
+        <is>
+          <t>Team plan $19/мес. 530 команд = $10K. Но риск: форматы могут унифицироваться сами.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="B10" s="11" t="inlineStr">
+        <is>
+          <t>MCP Server Health Monitor</t>
+        </is>
+      </c>
+      <c r="C10" s="11" t="inlineStr">
+        <is>
+          <t>MCP Ops</t>
+        </is>
+      </c>
+      <c r="D10" s="11" t="inlineStr">
+        <is>
+          <t>MCP-сервера падают в продакшене без предупреждения. Runtime failures у большинства серверов. Нет uptime monitoring для MCP.</t>
+        </is>
+      </c>
+      <c r="E10" s="11" t="inlineStr">
+        <is>
+          <t>UptimeRobot, Better Uptime (не понимают MCP протокол)</t>
+        </is>
+      </c>
+      <c r="F10" s="11" t="inlineStr">
+        <is>
+          <t>Обычные uptime мониторы проверяют HTTP. MCP — другой протокол (stdio/SSE). Нужна MCP-специфичная проверка.</t>
+        </is>
+      </c>
+      <c r="G10" s="11" t="inlineStr">
+        <is>
+          <t>Монитор: пинг MCP-серверов (list_tools, пробные вызовы), дашборд статусов, алерты</t>
+        </is>
+      </c>
+      <c r="H10" s="11" t="inlineStr">
+        <is>
+          <t>Hosted monitoring, status page для клиентов, SLA отчёты, интеграция с PagerDuty/Slack, история инцидентов</t>
+        </is>
+      </c>
+      <c r="I10" s="11" t="inlineStr">
+        <is>
+          <t>TypeScript/Go, Cron, MCP SDK, React dashboard</t>
+        </is>
+      </c>
+      <c r="J10" s="11" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+      <c r="K10" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="L10" s="11" t="inlineStr">
+        <is>
+          <t>Средний</t>
+        </is>
+      </c>
+      <c r="M10" s="11" t="inlineStr">
+        <is>
+          <t>Нулевой</t>
+        </is>
+      </c>
+      <c r="N10" s="11" t="inlineStr">
+        <is>
+          <t>Компании с MCP-серверами в продакшене. DevOps/SRE команды.</t>
+        </is>
+      </c>
+      <c r="O10" s="11" t="inlineStr">
+        <is>
+          <t>$29/мес на 10 серверов. 350 команд = $10K. Аналог Better Uptime но для MCP.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" s="11" t="inlineStr">
+        <is>
+          <t>Cursor Rules Auto-Generator</t>
+        </is>
+      </c>
+      <c r="C11" s="11" t="inlineStr">
+        <is>
+          <t>Agent DX</t>
+        </is>
+      </c>
+      <c r="D11" s="11" t="inlineStr">
+        <is>
+          <t>Библиотеки на npm/pip не имеют .cursor/rules. AI-агенты делают ошибки потому что не знают API библиотеки.</t>
+        </is>
+      </c>
+      <c r="E11" s="11" t="inlineStr">
+        <is>
+          <t>RuleBox.ai (ручные rules)</t>
+        </is>
+      </c>
+      <c r="F11" s="11" t="inlineStr">
+        <is>
+          <t>Всё ручное. Никто не генерирует rules автоматически из docs/types библиотеки.</t>
+        </is>
+      </c>
+      <c r="G11" s="11" t="inlineStr">
+        <is>
+          <t>CLI: `rules-gen react-query` → генерирует .cursor/rules из npm docs + TypeScript types</t>
+        </is>
+      </c>
+      <c r="H11" s="11" t="inlineStr">
+        <is>
+          <t>Cloud-версия: авто-обновление при релизах библиотеки, кастомные rules поверх, team sharing</t>
+        </is>
+      </c>
+      <c r="I11" s="11" t="inlineStr">
+        <is>
+          <t>TypeScript, AST parser, LLM API (для генерации), npm registry API</t>
+        </is>
+      </c>
+      <c r="J11" s="11" t="inlineStr">
+        <is>
+          <t>2-3</t>
+        </is>
+      </c>
+      <c r="K11" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="L11" s="11" t="inlineStr">
+        <is>
+          <t>Средний</t>
+        </is>
+      </c>
+      <c r="M11" s="11" t="inlineStr">
+        <is>
+          <t>Низкий (использует LLM, но не конкурирует)</t>
+        </is>
+      </c>
+      <c r="N11" s="11" t="inlineStr">
+        <is>
+          <t>Все разработчики использующие Cursor/Cline. Авторы библиотек.</t>
+        </is>
+      </c>
+      <c r="O11" s="11" t="inlineStr">
+        <is>
+          <t>Pro $9/мес (auto-update). 1100 юзеров = $10K. Огромный TAM (2M+ npm packages).</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B12" s="11" t="inlineStr">
+        <is>
+          <t>MCP Server Boilerplate / SDK+</t>
+        </is>
+      </c>
+      <c r="C12" s="11" t="inlineStr">
+        <is>
+          <t>MCP Tooling</t>
+        </is>
+      </c>
+      <c r="D12" s="11" t="inlineStr">
+        <is>
+          <t>Написать MCP-сервер с нуля сложно: auth, error handling, logging, testing, deployment. Офиц. SDK минимальный.</t>
+        </is>
+      </c>
+      <c r="E12" s="11" t="inlineStr">
+        <is>
+          <t>FastMCP (Python, базовый), офиц. SDK (минимальный)</t>
+        </is>
+      </c>
+      <c r="F12" s="11" t="inlineStr">
+        <is>
+          <t>FastMCP — только Python, без auth/deploy/monitoring. Офиц. SDK — низкоуровневый. Нет batteries-included решения.</t>
+        </is>
+      </c>
+      <c r="G12" s="11" t="inlineStr">
+        <is>
+          <t>Batteries-included фреймворк: auth, validation, logging, error handling, health checks, CLI scaffold</t>
+        </is>
+      </c>
+      <c r="H12" s="11" t="inlineStr">
+        <is>
+          <t>Pro templates (готовые сервера для Stripe/Notion/Slack), hosted deploy, monitoring dashboard</t>
+        </is>
+      </c>
+      <c r="I12" s="11" t="inlineStr">
+        <is>
+          <t>TypeScript, MCP SDK, Zod, CLI (create-mcp-server)</t>
+        </is>
+      </c>
+      <c r="J12" s="11" t="inlineStr">
+        <is>
+          <t>4-5</t>
+        </is>
+      </c>
+      <c r="K12" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="L12" s="11" t="inlineStr">
+        <is>
+          <t>Средний-высокий</t>
+        </is>
+      </c>
+      <c r="M12" s="11" t="inlineStr">
+        <is>
+          <t>Нулевой</t>
+        </is>
+      </c>
+      <c r="N12" s="11" t="inlineStr">
+        <is>
+          <t>MCP-разработчики которые строят сервера для своих продуктов/компаний</t>
+        </is>
+      </c>
+      <c r="O12" s="11" t="inlineStr">
+        <is>
+          <t>Pro templates $49/шт + hosted deploy $29/мес. Аналог create-t3-app но для MCP.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B13" s="11" t="inlineStr">
+        <is>
+          <t>LLM Gateway Lite (OSS)</t>
+        </is>
+      </c>
+      <c r="C13" s="11" t="inlineStr">
+        <is>
+          <t>Agent Infra</t>
+        </is>
+      </c>
+      <c r="D13" s="11" t="inlineStr">
+        <is>
+          <t>Компании используют 3-4 LLM провайдера одновременно. Нужно: fallback, роутинг, кеш, единый billing.</t>
+        </is>
+      </c>
+      <c r="E13" s="11" t="inlineStr">
+        <is>
+          <t>Portkey (closed), LiteLLM (broad), Bifrost (infra-heavy)</t>
+        </is>
+      </c>
+      <c r="F13" s="11" t="inlineStr">
+        <is>
+          <t>Portkey — закрытый. LiteLLM — сложный и тяжёлый. Нет лёгкого OSS прокси 'поставил за 5 минут'.</t>
+        </is>
+      </c>
+      <c r="G13" s="11" t="inlineStr">
+        <is>
+          <t>Lightweight proxy: unified API, fallback между провайдерами, semantic cache, логирование</t>
+        </is>
+      </c>
+      <c r="H13" s="11" t="inlineStr">
+        <is>
+          <t>Team dashboard, smart routing (дешёвая модель для простых запросов), spend limits, PII masking, hosted</t>
+        </is>
+      </c>
+      <c r="I13" s="11" t="inlineStr">
+        <is>
+          <t>TypeScript/Go, HTTP Proxy, Redis (cache), React dashboard</t>
+        </is>
+      </c>
+      <c r="J13" s="11" t="inlineStr">
+        <is>
+          <t>4-6</t>
+        </is>
+      </c>
+      <c r="K13" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="L13" s="11" t="inlineStr">
+        <is>
+          <t>Высокий</t>
+        </is>
+      </c>
+      <c r="M13" s="11" t="inlineStr">
+        <is>
+          <t>Нулевой</t>
+        </is>
+      </c>
+      <c r="N13" s="11" t="inlineStr">
+        <is>
+          <t>AI-стартапы, команды с multi-provider setup (GPT + Claude + Gemini)</t>
+        </is>
+      </c>
+      <c r="O13" s="11" t="inlineStr">
+        <is>
+          <t>Hosted $49/мес. 200 команд = $10K. Аналог Nginx но для LLM API.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="12">
+        <f>== РЫНОЧНЫЙ КОНТЕКСТ ===</f>
+        <v/>
+      </c>
+      <c r="B16" s="12" t="n"/>
+      <c r="C16" s="12" t="n"/>
+      <c r="D16" s="12" t="n"/>
+      <c r="E16" s="12" t="n"/>
+      <c r="F16" s="12" t="n"/>
+      <c r="G16" s="12" t="n"/>
+      <c r="H16" s="12" t="n"/>
+      <c r="I16" s="12" t="n"/>
+      <c r="J16" s="12" t="n"/>
+      <c r="K16" s="12" t="n"/>
+      <c r="L16" s="12" t="n"/>
+      <c r="M16" s="12" t="n"/>
+      <c r="N16" s="12" t="n"/>
+      <c r="O16" s="12" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="13" t="inlineStr">
+        <is>
+          <t>Метрика</t>
+        </is>
+      </c>
+      <c r="B17" s="13" t="inlineStr">
+        <is>
+          <t>Значение</t>
+        </is>
+      </c>
+      <c r="C17" s="13" t="inlineStr">
+        <is>
+          <t>Источник</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>MCP SDK скачиваний/месяц</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>97 млн</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>npm / MCP docs</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>MCP-серверов в публичном реестре</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>10,000+</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>MCP Registry</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>MCP-серверов с build failures</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>79%</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>NimbleBrain</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>MCP-серверов не деплоятся</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>20.7%</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NimbleBrain</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Cursor пользователей</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2M+</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Cursor blog</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Cline GitHub stars</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>58,200</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>GitHub</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>GitHub Copilot SDK</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Technical Preview (янв 2026)</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>GitHub Blog</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>MCP SDK языков</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>10+ (TS, Python, Go, Rust, Java, ...)</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>MCP GitHub</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>LLM API снижение цен за 16 мес</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>-83%</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>OpenAI / FutureSearch</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>AI M&amp;A сделок за 7 мес 2025</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>$55.3B</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>PYMNTS</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="14" t="n"/>
+      <c r="B28" s="14" t="n"/>
+      <c r="C28" s="14" t="n"/>
+      <c r="D28" s="14" t="n"/>
+      <c r="E28" s="14" t="n"/>
+      <c r="F28" s="14" t="inlineStr">
+        <is>
+          <t>Идея</t>
+        </is>
+      </c>
+      <c r="G28" s="14" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="H28" s="14" t="n"/>
+      <c r="I28" s="14" t="inlineStr">
+        <is>
+          <t>Категория</t>
+        </is>
+      </c>
+      <c r="J28" s="14" t="inlineStr">
+        <is>
+          <t>Кол-во</t>
+        </is>
+      </c>
+      <c r="K28" s="14" t="n"/>
+      <c r="L28" s="14" t="n"/>
+      <c r="M28" s="14" t="n"/>
+      <c r="N28" s="14" t="n"/>
+      <c r="O28" s="14" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="15">
+        <f>== ИТОГОВЫЙ РЕЙТИНГ ===</f>
+        <v/>
+      </c>
+      <c r="B29" s="15" t="n"/>
+      <c r="C29" s="15" t="n"/>
+      <c r="D29" s="15" t="n"/>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>MCP Test</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>9</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>MCP Tooling</t>
+        </is>
+      </c>
+      <c r="J29" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="16" t="inlineStr">
+        <is>
+          <t>Ранг</t>
+        </is>
+      </c>
+      <c r="B30" s="16" t="inlineStr">
+        <is>
+          <t>Идея</t>
+        </is>
+      </c>
+      <c r="C30" s="16" t="inlineStr">
+        <is>
+          <t>Score (1-10)</t>
+        </is>
+      </c>
+      <c r="D30" s="16" t="inlineStr">
+        <is>
+          <t>Почему этот ранг</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Cost Tracker</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>9</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Agent Observability</t>
+        </is>
+      </c>
+      <c r="J30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>1</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>MCP Test Framework</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>9</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Быстрый MVP (3-4 нед) + нулевая конкуренция + понятная боль (79% серверов сломаны). Можно сразу показать ценность: прогнал тесты на топ-100 MCP серверах, опубликовал результаты — виральный контент.</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>OpenAPI↔MCP</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>8</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>MCP Security</t>
+        </is>
+      </c>
+      <c r="J31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>AI Agent Cost Tracker</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>9</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Самый быстрый MVP (2-3 нед) + боль у всех разработчиков (счета за API растут). Огромный TAM: каждый кто использует LLM API. Launch на HN/Twitter.</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Auth Middleware</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>8</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Agent DX</t>
+        </is>
+      </c>
+      <c r="J32" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>3</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>OpenAPI ↔ MCP конвертер</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>8</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Понятный результат (скормил → получил) + огромный рынок (тысячи OpenAPI specs) + enterprise необходимость. Auto-sync — очевидная платная фича.</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Package Manager</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>7</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>MCP Ops</t>
+        </is>
+      </c>
+      <c r="J33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>4</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>MCP Auth Middleware</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>8</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Высокий revenue (enterprise платит за security) + реальная проблема (Kong/Red Hat пишут гайды — значит боль реальна). Но MVP сложнее.</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Rules Gen</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>7</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Agent Infra</t>
+        </is>
+      </c>
+      <c r="J34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>5</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>MCP Package Manager</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>7</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Самый высокий ceiling (может стать стандартом как npm), но самый долгий MVP (6-8 нед) и риск что Anthropic/официальный реестр сделает это сам.</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Boilerplate</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>6</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Cursor Rules Auto-Generator</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>7</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Очень быстрый MVP (2-3 нед) + огромный TAM (2M+ npm пакетов). Но низкая цена ($9/мес) и риск что Cursor сам добавит это.</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Health Monitor</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>7</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>MCP Server Boilerplate</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>7</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Понятный продукт (create-mcp-server), но официальные SDK улучшаются и могут поглотить эту нишу. FastMCP уже есть для Python.</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Config Manager</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>8</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>MCP Server Health Monitor</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>6</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Нужно компаниям с MCP в продакшене — но таких пока мало. Рынок растёт, но сегодня рано.</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>LLM Gateway</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="17" t="n">
+        <v>9</v>
+      </c>
+      <c r="B39" s="17" t="inlineStr">
+        <is>
+          <t>Agent Config Manager</t>
+        </is>
+      </c>
+      <c r="C39" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="D39" s="17" t="inlineStr">
+        <is>
+          <t>Боль реальна, но риск что форматы унифицируются (AGENTS.md становится стандартом — и продукт не нужен).</t>
+        </is>
+      </c>
+      <c r="E39" s="17" t="n"/>
+      <c r="F39" s="17" t="n"/>
+      <c r="G39" s="17" t="n"/>
+      <c r="H39" s="17" t="n"/>
+      <c r="I39" s="17" t="n"/>
+      <c r="J39" s="17" t="n"/>
+      <c r="K39" s="17" t="n"/>
+      <c r="L39" s="17" t="n"/>
+      <c r="M39" s="17" t="n"/>
+      <c r="N39" s="17" t="n"/>
+      <c r="O39" s="17" t="n"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="18" t="n">
+        <v>10</v>
+      </c>
+      <c r="B40" s="18" t="inlineStr">
+        <is>
+          <t>LLM Gateway Lite</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>5</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Сильная конкуренция (LiteLLM, Portkey, Bifrost). Длинный MVP. Но если сделать именно 'лёгкий' (5 мин установка) — есть шанс.</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="11" t="n"/>
+      <c r="B41" s="11" t="n"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="11">
+        <f>== СТРАТЕГИИ ЗАПУСКА ===</f>
+        <v/>
+      </c>
+      <c r="B42" s="11" t="n"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="11" t="inlineStr">
+        <is>
+          <t>Стратегия</t>
+        </is>
+      </c>
+      <c r="B43" s="11" t="inlineStr">
+        <is>
+          <t>Описание</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="11" t="inlineStr">
+        <is>
+          <t>Быстрый старт (2-4 нед)</t>
+        </is>
+      </c>
+      <c r="B44" s="11" t="inlineStr">
+        <is>
+          <t>#2 Cost Tracker или #8 Rules Generator. Минимальный MVP, launch на HN/Twitter/Reddit. Сбор фидбэка и первых юзеров.</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Сбалансированный (3-5 нед)</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>#1 MCP Test Framework или #5 OpenAPI↔MCP. Лучший баланс скорости/риска/revenue. Launch + виральный контент (тесты топ-100 MCP серверов).</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="19" t="inlineStr">
+        <is>
+          <t>Амбициозный (6-8 нед)</t>
+        </is>
+      </c>
+      <c r="B46" s="19" t="inlineStr">
+        <is>
+          <t>#3 MCP Package Manager или #4 Auth Middleware. Максимальный ceiling, но долгий путь и больше риска. Нужна сильная вера в MCP экосистему.</t>
+        </is>
+      </c>
+      <c r="C46" s="19" t="n"/>
+      <c r="D46" s="19" t="n"/>
+      <c r="E46" s="19" t="n"/>
+      <c r="F46" s="19" t="n"/>
+      <c r="G46" s="19" t="n"/>
+      <c r="H46" s="19" t="n"/>
+      <c r="I46" s="19" t="n"/>
+      <c r="J46" s="19" t="n"/>
+      <c r="K46" s="19" t="n"/>
+      <c r="L46" s="19" t="n"/>
+      <c r="M46" s="19" t="n"/>
+      <c r="N46" s="19" t="n"/>
+      <c r="O46" s="19" t="n"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="20" t="inlineStr">
+        <is>
+          <t>Комбо-план</t>
+        </is>
+      </c>
+      <c r="B47" s="20" t="inlineStr">
+        <is>
+          <t>Начать с #1 (Test Framework) → добавить #7 (Health Monitor) → вырасти в полную MCP DevOps платформу. Один бренд, несколько продуктов.</t>
+        </is>
+      </c>
+      <c r="C47" s="20" t="n"/>
+      <c r="D47" s="20" t="n"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="11" t="n"/>
+      <c r="B48" s="11" t="n"/>
+      <c r="C48" s="11" t="n"/>
+      <c r="D48" s="11" t="n"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="11">
+        <f>== ПОЧЕМУ ЭТО БЕЗОПАСНЕЕ AI-ОБЁРТОК ===</f>
+        <v/>
+      </c>
+      <c r="B49" s="11" t="n"/>
+      <c r="C49" s="11" t="n"/>
+      <c r="D49" s="11" t="n"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="11" t="inlineStr">
+        <is>
+          <t>Критерий</t>
+        </is>
+      </c>
+      <c r="B50" s="11" t="inlineStr">
+        <is>
+          <t>AI-обёртка</t>
+        </is>
+      </c>
+      <c r="C50" s="11" t="inlineStr">
+        <is>
+          <t>AI Infra (MCP/DevTools)</t>
+        </is>
+      </c>
+      <c r="D50" s="11" t="n"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="11" t="inlineStr">
+        <is>
+          <t>Moat</t>
+        </is>
+      </c>
+      <c r="B51" s="11" t="inlineStr">
+        <is>
+          <t>Никакого</t>
+        </is>
+      </c>
+      <c r="C51" s="11" t="inlineStr">
+        <is>
+          <t>Community + ecosystem + integrations</t>
+        </is>
+      </c>
+      <c r="D51" s="11" t="n"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="11" t="inlineStr">
+        <is>
+          <t>Gross margin</t>
+        </is>
+      </c>
+      <c r="B52" s="11" t="inlineStr">
+        <is>
+          <t>25-60%</t>
+        </is>
+      </c>
+      <c r="C52" s="11" t="inlineStr">
+        <is>
+          <t>80-90% (нет LLM API costs)</t>
+        </is>
+      </c>
+      <c r="D52" s="11" t="n"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="11" t="inlineStr">
+        <is>
+          <t>Риск от OpenAI</t>
+        </is>
+      </c>
+      <c r="B53" s="11" t="inlineStr">
+        <is>
+          <t>Высокий (убьют фичей)</t>
+        </is>
+      </c>
+      <c r="C53" s="11" t="inlineStr">
+        <is>
+          <t>Нулевой (OpenAI не делает DevTools)</t>
+        </is>
+      </c>
+      <c r="D53" s="11" t="n"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Маркетинг</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Платный (ads, outreach)</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Бесплатный (GitHub, npm, HN)</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Пример провала</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Jasper, Phind, CodeParrot</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Редко — если community есть, проект живёт</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Пример успеха</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Почти нет</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Sidekiq $10M, Supabase $5B, PostHog $9.5M</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Time to copy</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>3-6 месяцев</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>1-2 года (нужна community)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add MCP Platform unified strategy sheet
New sheet "MCP Platform" with complete startup plan:
- 5 platform features (Registry, Testing, Auth, Health, OpenAPI converter)
- Phase-by-phase roadmap (0-4, weeks 1-16)
- Feature interconnection map
- Pricing tiers (Free/Pro/Team/Enterprise)
- Path to $10K MRR scenarios
- Why testing first: virality, simplicity, bridge to registry
- Honest recommendation with actionable next steps

Made-with: Cursor
</commit_message>
<xml_diff>
--- a/yc_startups_analysis.xlsx
+++ b/yc_startups_analysis.xlsx
@@ -13,6 +13,7 @@
     <sheet name="Идеи для тебя" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Риски AI-обёрток" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="AI Infra идеи" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="MCP Platform" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -22,7 +23,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="8">
+  <fonts count="14">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -58,8 +59,35 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="FF1B5E20"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="FFF57F17"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="FF1B5E20"/>
+      <sz val="14"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="22">
     <fill>
       <patternFill/>
     </fill>
@@ -156,6 +184,36 @@
         <bgColor rgb="FFC62828"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1A237E"/>
+        <bgColor rgb="FF1A237E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF283593"/>
+        <bgColor rgb="FF283593"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3949AB"/>
+        <bgColor rgb="FF3949AB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF9C4"/>
+        <bgColor rgb="00FFF9C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8EAF6"/>
+        <bgColor rgb="FFE8EAF6"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -169,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -201,6 +259,25 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -9154,4 +9231,943 @@
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="21">
+        <f>== MCP PLATFORM: ЕДИНАЯ ПЛАТФОРМА ДЛЯ MCP-ЭКОСИСТЕМЫ ===</f>
+        <v/>
+      </c>
+      <c r="B1" s="21" t="n"/>
+      <c r="C1" s="21" t="n"/>
+      <c r="D1" s="21" t="n"/>
+      <c r="E1" s="21" t="n"/>
+      <c r="F1" s="21" t="n"/>
+      <c r="G1" s="21" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="22" t="inlineStr">
+        <is>
+          <t>Название (рабочее)</t>
+        </is>
+      </c>
+      <c r="B3" s="11" t="inlineStr">
+        <is>
+          <t>mcpkit или mcp-tools или mcphub</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="22" t="inlineStr">
+        <is>
+          <t>Однострочник</t>
+        </is>
+      </c>
+      <c r="B4" s="11" t="inlineStr">
+        <is>
+          <t>npm + Jest + Auth proxy — но для MCP</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="22" t="inlineStr">
+        <is>
+          <t>Почему одна платформа</t>
+        </is>
+      </c>
+      <c r="B5" s="11" t="inlineStr">
+        <is>
+          <t>Один бренд = больше доверия. Клиент пришёл за тестами — остался ради registry и auth. Cross-sell встроен в продукт.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="23">
+        <f>== ФИЧИ ПЛАТФОРМЫ ===</f>
+        <v/>
+      </c>
+      <c r="B7" s="23" t="n"/>
+      <c r="C7" s="23" t="n"/>
+      <c r="D7" s="23" t="n"/>
+      <c r="E7" s="23" t="n"/>
+      <c r="F7" s="23" t="n"/>
+      <c r="G7" s="23" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="24" t="inlineStr">
+        <is>
+          <t>Фича</t>
+        </is>
+      </c>
+      <c r="B8" s="24" t="inlineStr">
+        <is>
+          <t>Что делает</t>
+        </is>
+      </c>
+      <c r="C8" s="24" t="inlineStr">
+        <is>
+          <t>Аналогия</t>
+        </is>
+      </c>
+      <c r="D8" s="24" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E8" s="24" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+      <c r="F8" s="24" t="inlineStr">
+        <is>
+          <t>Приоритет</t>
+        </is>
+      </c>
+      <c r="G8" s="24" t="inlineStr">
+        <is>
+          <t>Недели до MVP</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="11" t="inlineStr">
+        <is>
+          <t>1. Registry + CLI</t>
+        </is>
+      </c>
+      <c r="B9" s="11" t="inlineStr">
+        <is>
+          <t>mcp install stripe — и MCP-сервер установлен, настроен, работает. mcp search — поиск по каталогу. mcp update — обновление всех серверов. Авто-конфиг для Cursor / Claude / Cline.</t>
+        </is>
+      </c>
+      <c r="C9" s="11" t="inlineStr">
+        <is>
+          <t>npm / Homebrew</t>
+        </is>
+      </c>
+      <c r="D9" s="11" t="inlineStr">
+        <is>
+          <t>Public registry, install, search, update, auto-config для всех агентов</t>
+        </is>
+      </c>
+      <c r="E9" s="11" t="inlineStr">
+        <is>
+          <t>Private registry для компаний (внутренние MCP-сервера), team management, аналитика использования</t>
+        </is>
+      </c>
+      <c r="F9" s="25" t="inlineStr">
+        <is>
+          <t>ЯДРО</t>
+        </is>
+      </c>
+      <c r="G9" s="11" t="inlineStr">
+        <is>
+          <t>4-5</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="11" t="inlineStr">
+        <is>
+          <t>2. Testing</t>
+        </is>
+      </c>
+      <c r="B10" s="11" t="inlineStr">
+        <is>
+          <t>mcp test ./server — автоматически проверяет: запускается ли сервер? отвечает на list_tools? совпадают ли типы? не падают ли инструменты? Снэпшоты ответов для регрессии.</t>
+        </is>
+      </c>
+      <c r="C10" s="11" t="inlineStr">
+        <is>
+          <t>Jest / pytest</t>
+        </is>
+      </c>
+      <c r="D10" s="11" t="inlineStr">
+        <is>
+          <t>Локальный CLI тест-раннер (запуск, валидация, снэпшоты, отчёт)</t>
+        </is>
+      </c>
+      <c r="E10" s="11" t="inlineStr">
+        <is>
+          <t>GitHub Action для CI/CD, badge 'MCP Verified' в registry, hosted dashboard с историей тестов</t>
+        </is>
+      </c>
+      <c r="F10" s="25" t="inlineStr">
+        <is>
+          <t>ЯДРО</t>
+        </is>
+      </c>
+      <c r="G10" s="11" t="inlineStr">
+        <is>
+          <t>2-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="11" t="inlineStr">
+        <is>
+          <t>3. Auth &amp; Security</t>
+        </is>
+      </c>
+      <c r="B11" s="11" t="inlineStr">
+        <is>
+          <t>mcp proxy — прокси между AI-агентом и MCP-сервером. Проверяет кто вызывает, что вызывает, логирует всё. Блокирует опасные вызовы.</t>
+        </is>
+      </c>
+      <c r="C11" s="11" t="inlineStr">
+        <is>
+          <t>Kong / Nginx но для MCP</t>
+        </is>
+      </c>
+      <c r="D11" s="11" t="inlineStr">
+        <is>
+          <t>API key auth, базовые логи, фильтрация tool calls</t>
+        </is>
+      </c>
+      <c r="E11" s="11" t="inlineStr">
+        <is>
+          <t>SSO (Okta/Azure AD), role-based access (кто какие tools может), audit trail, PII фильтр, compliance отчёты</t>
+        </is>
+      </c>
+      <c r="F11" s="26" t="inlineStr">
+        <is>
+          <t>ФАЗА 2</t>
+        </is>
+      </c>
+      <c r="G11" s="11" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="11" t="inlineStr">
+        <is>
+          <t>4. Health Monitor</t>
+        </is>
+      </c>
+      <c r="B12" s="11" t="inlineStr">
+        <is>
+          <t>mcp status — дашборд: какие сервера живы, какие упали, время отклика, алерты в Slack если сервер сломался.</t>
+        </is>
+      </c>
+      <c r="C12" s="11" t="inlineStr">
+        <is>
+          <t>UptimeRobot но для MCP</t>
+        </is>
+      </c>
+      <c r="D12" s="11" t="inlineStr">
+        <is>
+          <t>Локальный пинг серверов, CLI статус</t>
+        </is>
+      </c>
+      <c r="E12" s="11" t="inlineStr">
+        <is>
+          <t>Hosted dashboard, Slack/email алерты, status page для клиентов, SLA отчёты</t>
+        </is>
+      </c>
+      <c r="F12" s="27" t="inlineStr">
+        <is>
+          <t>ФАЗА 3</t>
+        </is>
+      </c>
+      <c r="G12" s="11" t="inlineStr">
+        <is>
+          <t>2-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="11" t="inlineStr">
+        <is>
+          <t>5. OpenAPI → MCP</t>
+        </is>
+      </c>
+      <c r="B13" s="11" t="inlineStr">
+        <is>
+          <t>mcp convert openapi.yaml — скормила OpenAPI spec любого API — получила готовый MCP-сервер. Не надо писать код.</t>
+        </is>
+      </c>
+      <c r="C13" s="11" t="inlineStr">
+        <is>
+          <t>Swagger Codegen но MCP→</t>
+        </is>
+      </c>
+      <c r="D13" s="11" t="inlineStr">
+        <is>
+          <t>CLI конвертер (openapi.yaml → MCP server)</t>
+        </is>
+      </c>
+      <c r="E13" s="11" t="inlineStr">
+        <is>
+          <t>Auto-sync (обновился API → авто-обновился MCP), кастомные правила</t>
+        </is>
+      </c>
+      <c r="F13" s="27" t="inlineStr">
+        <is>
+          <t>БОНУС</t>
+        </is>
+      </c>
+      <c r="G13" s="11" t="inlineStr">
+        <is>
+          <t>2-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="23">
+        <f>== РОДМАП: ЧТО КОГДА ДЕЛАТЬ ===</f>
+        <v/>
+      </c>
+      <c r="B16" s="23" t="n"/>
+      <c r="C16" s="23" t="n"/>
+      <c r="D16" s="23" t="n"/>
+      <c r="E16" s="23" t="n"/>
+      <c r="F16" s="23" t="n"/>
+      <c r="G16" s="23" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="24" t="inlineStr">
+        <is>
+          <t>Фаза</t>
+        </is>
+      </c>
+      <c r="B17" s="24" t="inlineStr">
+        <is>
+          <t>Срок</t>
+        </is>
+      </c>
+      <c r="C17" s="24" t="inlineStr">
+        <is>
+          <t>Что делаем</t>
+        </is>
+      </c>
+      <c r="D17" s="24" t="inlineStr">
+        <is>
+          <t>Результат</t>
+        </is>
+      </c>
+      <c r="E17" s="24" t="inlineStr">
+        <is>
+          <t>Монетизация</t>
+        </is>
+      </c>
+      <c r="F17" s="24" t="inlineStr">
+        <is>
+          <t>Метрика успеха</t>
+        </is>
+      </c>
+      <c r="G17" s="24" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="11" t="inlineStr">
+        <is>
+          <t>Фаза 0: Валидация</t>
+        </is>
+      </c>
+      <c r="B18" s="11" t="inlineStr">
+        <is>
+          <t>Неделя 1</t>
+        </is>
+      </c>
+      <c r="C18" s="11" t="inlineStr">
+        <is>
+          <t>Landing page + waitlist. Пост на HN/Twitter: 'Мы протестировали топ-100 MCP серверов, 79 сломаны' + таблица результатов. Виральный контент.</t>
+        </is>
+      </c>
+      <c r="D18" s="11" t="inlineStr">
+        <is>
+          <t>Понимание спроса. Первые email в waitlist.</t>
+        </is>
+      </c>
+      <c r="E18" s="11" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="F18" s="11" t="inlineStr">
+        <is>
+          <t>100+ в waitlist = go</t>
+        </is>
+      </c>
+      <c r="G18" s="11" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="11" t="inlineStr">
+        <is>
+          <t>Фаза 1: mcp test</t>
+        </is>
+      </c>
+      <c r="B19" s="11" t="inlineStr">
+        <is>
+          <t>Недели 2-4</t>
+        </is>
+      </c>
+      <c r="C19" s="11" t="inlineStr">
+        <is>
+          <t>CLI тест-раннер. Запуск MCP-сервера, проверка list_tools, валидация Zod-схем, снэпшоты ответов, отчёт в терминале. Open source.</t>
+        </is>
+      </c>
+      <c r="D19" s="11" t="inlineStr">
+        <is>
+          <t>Первый продукт. GitHub stars. Комьюнити.</t>
+        </is>
+      </c>
+      <c r="E19" s="11" t="inlineStr">
+        <is>
+          <t>Free (OSS)</t>
+        </is>
+      </c>
+      <c r="F19" s="11" t="inlineStr">
+        <is>
+          <t>500+ GitHub stars, 50+ weekly npm installs</t>
+        </is>
+      </c>
+      <c r="G19" s="11" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="inlineStr">
+        <is>
+          <t>Фаза 2: mcp install</t>
+        </is>
+      </c>
+      <c r="B20" s="11" t="inlineStr">
+        <is>
+          <t>Недели 5-8</t>
+        </is>
+      </c>
+      <c r="C20" s="11" t="inlineStr">
+        <is>
+          <t>CLI: mcp install stripe, mcp search, mcp update. Public registry. Авто-конфиг для Cursor/Claude/Cline. Интеграция с mcp test: сервер в registry показывает статус тестов.</t>
+        </is>
+      </c>
+      <c r="D20" s="11" t="inlineStr">
+        <is>
+          <t>Ядро платформы. Привычка у юзеров.</t>
+        </is>
+      </c>
+      <c r="E20" s="11" t="inlineStr">
+        <is>
+          <t>Free registry + Paid private registries ($49/мес)</t>
+        </is>
+      </c>
+      <c r="F20" s="11" t="inlineStr">
+        <is>
+          <t>200+ MCP-серверов в registry</t>
+        </is>
+      </c>
+      <c r="G20" s="11" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="11" t="inlineStr">
+        <is>
+          <t>Фаза 3: mcp proxy (auth)</t>
+        </is>
+      </c>
+      <c r="B21" s="11" t="inlineStr">
+        <is>
+          <t>Недели 9-12</t>
+        </is>
+      </c>
+      <c r="C21" s="11" t="inlineStr">
+        <is>
+          <t>Прокси между агентом и MCP: API key auth, логи всех вызовов, фильтрация опасных tool calls. Интеграция с registry: mcp install --with-proxy.</t>
+        </is>
+      </c>
+      <c r="D21" s="11" t="inlineStr">
+        <is>
+          <t>Enterprise клиенты. Высокий revenue.</t>
+        </is>
+      </c>
+      <c r="E21" s="11" t="inlineStr">
+        <is>
+          <t>Free self-hosted + Paid hosted ($99-199/мес)</t>
+        </is>
+      </c>
+      <c r="F21" s="11" t="inlineStr">
+        <is>
+          <t>10+ платящих компаний</t>
+        </is>
+      </c>
+      <c r="G21" s="11" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="11" t="inlineStr">
+        <is>
+          <t>Фаза 4: Dashboard</t>
+        </is>
+      </c>
+      <c r="B22" s="11" t="inlineStr">
+        <is>
+          <t>Недели 13-16</t>
+        </is>
+      </c>
+      <c r="C22" s="11" t="inlineStr">
+        <is>
+          <t>Web-панель: все сервера команды, статусы тестов, здоровье, логи auth, аналитика. Всё в одном месте.</t>
+        </is>
+      </c>
+      <c r="D22" s="11" t="inlineStr">
+        <is>
+          <t>Полноценная платформа. Можно поднимать цены.</t>
+        </is>
+      </c>
+      <c r="E22" s="11" t="inlineStr">
+        <is>
+          <t>Team plan $149/мес (all-in-one)</t>
+        </is>
+      </c>
+      <c r="F22" s="11" t="inlineStr">
+        <is>
+          <t>$10K MRR</t>
+        </is>
+      </c>
+      <c r="G22" s="11" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="23">
+        <f>== ПОЧЕМУ ТЕСТИРОВАНИЕ — ЛУЧШИЙ СТАРТ ===</f>
+        <v/>
+      </c>
+      <c r="B24" s="23" t="n"/>
+      <c r="C24" s="23" t="n"/>
+      <c r="D24" s="23" t="n"/>
+      <c r="E24" s="23" t="n"/>
+      <c r="F24" s="23" t="n"/>
+      <c r="G24" s="23" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="28" t="inlineStr">
+        <is>
+          <t>Причина</t>
+        </is>
+      </c>
+      <c r="B25" s="11" t="inlineStr">
+        <is>
+          <t>Объяснение</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="28" t="inlineStr">
+        <is>
+          <t>1. Виральность встроена в продукт</t>
+        </is>
+      </c>
+      <c r="B26" s="11" t="inlineStr">
+        <is>
+          <t>Прогоняешь mcp test на топ-100 серверов, публикуешь таблицу результатов — это контент который разойдётся сам. 'Мы протестировали 100 MCP серверов — 79 сломаны' = заголовок который читают.</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="28" t="inlineStr">
+        <is>
+          <t>2. Самый простой MVP</t>
+        </is>
+      </c>
+      <c r="B27" s="11" t="inlineStr">
+        <is>
+          <t>2-3 недели. Не нужен сервер, база данных, UI. Просто CLI который запускает MCP-сервер и проверяет его. Publish на npm.</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="28" t="inlineStr">
+        <is>
+          <t>3. Натуральный мост к registry</t>
+        </is>
+      </c>
+      <c r="B28" s="11" t="inlineStr">
+        <is>
+          <t>Если ты уже тестируешь сервера — логично что у тебя есть registry проверенных. badge 'Verified by mcpkit' = доверие. Registry становится естественным продолжением.</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="28" t="inlineStr">
+        <is>
+          <t>4. Обратная связь бесплатно</t>
+        </is>
+      </c>
+      <c r="B29" s="11" t="inlineStr">
+        <is>
+          <t>Люди открывают issues: 'mcp test не поддерживает X' = ты узнаёшь что нужно рынку без кастдевов.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="28" t="inlineStr">
+        <is>
+          <t>5. Anthropic не сделает это</t>
+        </is>
+      </c>
+      <c r="B30" s="11" t="inlineStr">
+        <is>
+          <t>Тестирование / DevOps — не их бизнес. Anthropic делает протокол. Тулинг делает community. Как Jest не сделан Facebook (хотя React их).</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="23">
+        <f>== КАК ФИЧИ СВЯЗАНЫ МЕЖДУ СОБОЙ ===</f>
+        <v/>
+      </c>
+      <c r="B32" s="23" t="n"/>
+      <c r="C32" s="23" t="n"/>
+      <c r="D32" s="23" t="n"/>
+      <c r="E32" s="23" t="n"/>
+      <c r="F32" s="23" t="n"/>
+      <c r="G32" s="23" t="n"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="28" t="inlineStr">
+        <is>
+          <t>Связка</t>
+        </is>
+      </c>
+      <c r="B33" s="11" t="inlineStr">
+        <is>
+          <t>Как работает</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="28" t="inlineStr">
+        <is>
+          <t>Test → Registry</t>
+        </is>
+      </c>
+      <c r="B34" s="11" t="inlineStr">
+        <is>
+          <t>Сервер публикуется в registry только если прошёл mcp test. Бейдж 'Verified' в каталоге. Как npm с встроенным CI.</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="28" t="inlineStr">
+        <is>
+          <t>Registry → Auth</t>
+        </is>
+      </c>
+      <c r="B35" s="11" t="inlineStr">
+        <is>
+          <t>При установке сервера можно сразу настроить proxy: `mcp install stripe --with-proxy`. Auth идёт 'out of the box'.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="28" t="inlineStr">
+        <is>
+          <t>Test → Health</t>
+        </is>
+      </c>
+      <c r="B36" s="11" t="inlineStr">
+        <is>
+          <t>Тесты запускаются периодически → health monitoring. Тот же код, но по cron. Если тест упал → алерт.</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="28" t="inlineStr">
+        <is>
+          <t>Auth → Health</t>
+        </is>
+      </c>
+      <c r="B37" s="11" t="inlineStr">
+        <is>
+          <t>Прокси логирует все вызовы → данные для health dashboard. Какой сервер медленный, какой падает, кто вызывает что.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="23">
+        <f>== ПРАЙСИНГ ===</f>
+        <v/>
+      </c>
+      <c r="B39" s="23" t="n"/>
+      <c r="C39" s="23" t="n"/>
+      <c r="D39" s="23" t="n"/>
+      <c r="E39" s="23" t="n"/>
+      <c r="F39" s="23" t="n"/>
+      <c r="G39" s="23" t="n"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="24" t="inlineStr">
+        <is>
+          <t>План</t>
+        </is>
+      </c>
+      <c r="B40" s="24" t="inlineStr">
+        <is>
+          <t>Цена/мес</t>
+        </is>
+      </c>
+      <c r="C40" s="24" t="inlineStr">
+        <is>
+          <t>Что включено</t>
+        </is>
+      </c>
+      <c r="D40" s="24" t="inlineStr">
+        <is>
+          <t>Целевой клиент</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="11" t="inlineStr">
+        <is>
+          <t>Free (OSS)</t>
+        </is>
+      </c>
+      <c r="B41" s="11" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="C41" s="11" t="inlineStr">
+        <is>
+          <t>CLI (test + install + search), public registry, 3 private сервера, базовый auth proxy</t>
+        </is>
+      </c>
+      <c r="D41" s="11" t="inlineStr">
+        <is>
+          <t>Инди-разработчики, опенсорс</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="11" t="inlineStr">
+        <is>
+          <t>Pro</t>
+        </is>
+      </c>
+      <c r="B42" s="11" t="inlineStr">
+        <is>
+          <t>$29/мес</t>
+        </is>
+      </c>
+      <c r="C42" s="11" t="inlineStr">
+        <is>
+          <t>Unlimited private сервера, GitHub Action для CI, badge Verified, история тестов</t>
+        </is>
+      </c>
+      <c r="D42" s="11" t="inlineStr">
+        <is>
+          <t>Небольшие команды, стартапы</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="11" t="inlineStr">
+        <is>
+          <t>Team</t>
+        </is>
+      </c>
+      <c r="B43" s="11" t="inlineStr">
+        <is>
+          <t>$99/мес</t>
+        </is>
+      </c>
+      <c r="C43" s="11" t="inlineStr">
+        <is>
+          <t>Pro + auth proxy с SSO, team management, аналитика, health dashboard, Slack алерты</t>
+        </is>
+      </c>
+      <c r="D43" s="11" t="inlineStr">
+        <is>
+          <t>Средние компании</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="11" t="inlineStr">
+        <is>
+          <t>Enterprise</t>
+        </is>
+      </c>
+      <c r="B44" s="11" t="inlineStr">
+        <is>
+          <t>$299/мес</t>
+        </is>
+      </c>
+      <c r="C44" s="11" t="inlineStr">
+        <is>
+          <t>Team + audit trail, compliance, SLA, PII filtering, custom policies, dedicated support</t>
+        </is>
+      </c>
+      <c r="D44" s="11" t="inlineStr">
+        <is>
+          <t>Enterprise (SOC2, HIPAA)</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="23">
+        <f>== ПУТЬ К $10K MRR ===</f>
+        <v/>
+      </c>
+      <c r="B46" s="23" t="n"/>
+      <c r="C46" s="23" t="n"/>
+      <c r="D46" s="23" t="n"/>
+      <c r="E46" s="23" t="n"/>
+      <c r="F46" s="23" t="n"/>
+      <c r="G46" s="23" t="n"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="24" t="inlineStr">
+        <is>
+          <t>Сценарий</t>
+        </is>
+      </c>
+      <c r="B47" s="24" t="inlineStr">
+        <is>
+          <t>Формула</t>
+        </is>
+      </c>
+      <c r="C47" s="24" t="inlineStr">
+        <is>
+          <t>Реалистичность</t>
+        </is>
+      </c>
+      <c r="D47" s="24" t="n"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="11" t="inlineStr">
+        <is>
+          <t>Консервативный</t>
+        </is>
+      </c>
+      <c r="B48" s="11" t="inlineStr">
+        <is>
+          <t>100 Pro ($29) + 30 Team ($99) + 5 Enterprise ($299) = $7,365/мес</t>
+        </is>
+      </c>
+      <c r="C48" s="11" t="inlineStr">
+        <is>
+          <t>Месяц 6-8</t>
+        </is>
+      </c>
+      <c r="D48" s="11" t="n"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="11" t="inlineStr">
+        <is>
+          <t>Оптимистичный</t>
+        </is>
+      </c>
+      <c r="B49" s="11" t="inlineStr">
+        <is>
+          <t>200 Pro ($29) + 50 Team ($99) + 10 Enterprise ($299) = $13,740/мес</t>
+        </is>
+      </c>
+      <c r="C49" s="11" t="inlineStr">
+        <is>
+          <t>Месяц 4-6</t>
+        </is>
+      </c>
+      <c r="D49" s="11" t="n"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="29">
+        <f>== МОЙ ЧЕСТНЫЙ СОВЕТ ===</f>
+        <v/>
+      </c>
+      <c r="B51" s="29" t="n"/>
+      <c r="C51" s="29" t="n"/>
+      <c r="D51" s="29" t="n"/>
+      <c r="E51" s="29" t="n"/>
+      <c r="F51" s="29" t="n"/>
+      <c r="G51" s="29" t="n"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="28" t="inlineStr">
+        <is>
+          <t>Тезис</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Объяснение</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="28" t="inlineStr">
+        <is>
+          <t>НАЧНИ С mcp test</t>
+        </is>
+      </c>
+      <c r="B53" s="11" t="inlineStr">
+        <is>
+          <t>Не с registry. Test — это 2-3 недели до первого юзера. Registry — 6-8 недель. За 3 недели у тебя будет OSS продукт + виральный пост + комьюнити.</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="28" t="inlineStr">
+        <is>
+          <t>Не строй всё сразу</t>
+        </is>
+      </c>
+      <c r="B54" s="11" t="inlineStr">
+        <is>
+          <t>Test → подожди фидбэк → Registry → Auth. Каждая фаза валидирует следующую.</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="28" t="inlineStr">
+        <is>
+          <t>Сделай Фазу 0 сегодня</t>
+        </is>
+      </c>
+      <c r="B55" s="11" t="inlineStr">
+        <is>
+          <t>Прогони ручной тест на 10 MCP-серверах. Запиши результаты. Опубликуй на HN/Twitter. Это займёт 2-3 часа и даст ответ: нужно ли это рынку?</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="28" t="inlineStr">
+        <is>
+          <t>Имя = важно</t>
+        </is>
+      </c>
+      <c r="B56" s="11" t="inlineStr">
+        <is>
+          <t>Забронируй npm-пакет и GitHub org сейчас: mcpkit, mcp-tools, mcphub, mcpx. Кто первый — того и бренд.</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="28" t="inlineStr">
+        <is>
+          <t>AI-wrapper риск = 0</t>
+        </is>
+      </c>
+      <c r="B57" s="11" t="inlineStr">
+        <is>
+          <t>Это инфраструктура, не обёртка. Не используешь LLM API. OpenAI/Anthropic не конкуренты — клиенты. Чем больше AI-агентов — тем больше MCP — тем больше нужна платформа.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add competitive analysis: platform vs official registry
Honest analysis of competing with Anthropic's official MCP registry:
- Why you can't beat it as a registry (protocol control, distribution, resources)
- Why you don't need to: historical parallels (JFrog $3B vs npm, GitLab $8B vs GitHub)
- Correct strategy: build ON TOP, not instead
- Risk matrix with probabilities and defenses
- Layer diagram: protocol > registry > DevOps > enterprise (your territory)

Made-with: Cursor
</commit_message>
<xml_diff>
--- a/yc_startups_analysis.xlsx
+++ b/yc_startups_analysis.xlsx
@@ -23,7 +23,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="14">
+  <fonts count="17">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -86,8 +86,22 @@
       <color rgb="FF1B5E20"/>
       <sz val="14"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="FFB71C1C"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="FFB71C1C"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="FF1B5E20"/>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="25">
     <fill>
       <patternFill/>
     </fill>
@@ -214,6 +228,24 @@
         <bgColor rgb="FFE8EAF6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB71C1C"/>
+        <bgColor rgb="FFB71C1C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFCDD2"/>
+        <bgColor rgb="00FFCDD2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1B5E20"/>
+        <bgColor rgb="FF1B5E20"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -227,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -278,6 +310,25 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -9239,7 +9290,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10167,6 +10218,646 @@
         </is>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" s="30">
+        <f>== ЧЕСТНЫЙ АНАЛИЗ: МОЖЕШЬ ЛИ ТЫ ПОБЕДИТЬ ОФИЦИАЛЬНЫЙ РЕЕСТР? ===</f>
+        <v/>
+      </c>
+      <c r="B60" s="30" t="n"/>
+      <c r="C60" s="30" t="n"/>
+      <c r="D60" s="30" t="n"/>
+      <c r="E60" s="30" t="n"/>
+      <c r="F60" s="30" t="n"/>
+      <c r="G60" s="30" t="n"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="31" t="inlineStr">
+        <is>
+          <t>Короткий ответ:</t>
+        </is>
+      </c>
+      <c r="B62" s="31" t="inlineStr">
+        <is>
+          <t>Нет. И не надо.</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="23">
+        <f>== ПОЧЕМУ НЕ ПОБЕДИШЬ КАК РЕЕСТР ===</f>
+        <v/>
+      </c>
+      <c r="B64" s="23" t="n"/>
+      <c r="C64" s="23" t="n"/>
+      <c r="D64" s="23" t="n"/>
+      <c r="E64" s="23" t="n"/>
+      <c r="F64" s="23" t="n"/>
+      <c r="G64" s="23" t="n"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="32" t="inlineStr">
+        <is>
+          <t>Причина</t>
+        </is>
+      </c>
+      <c r="B65" s="32" t="inlineStr">
+        <is>
+          <t>Объяснение</t>
+        </is>
+      </c>
+      <c r="C65" s="32" t="inlineStr">
+        <is>
+          <t>Насколько критично</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="11" t="inlineStr">
+        <is>
+          <t>Anthropic контролирует протокол</t>
+        </is>
+      </c>
+      <c r="B66" s="11" t="inlineStr">
+        <is>
+          <t>Они меняют spec — ты догоняешь. Они добавили streamable HTTP в марте 2025 — всем пришлось обновляться. Твой реестр всегда будет вторым.</t>
+        </is>
+      </c>
+      <c r="C66" s="33" t="inlineStr">
+        <is>
+          <t>КРИТИЧНО</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="11" t="inlineStr">
+        <is>
+          <t>Авторы публикуются там первыми</t>
+        </is>
+      </c>
+      <c r="B67" s="11" t="inlineStr">
+        <is>
+          <t>Если ты Stripe и делаешь MCP-сервер — ты публикуешься в официальном реестре, не в стороннем. Это как с npm: никто не публикует пакет сначала в альтернативный registry.</t>
+        </is>
+      </c>
+      <c r="C67" s="33" t="inlineStr">
+        <is>
+          <t>КРИТИЧНО</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="11" t="inlineStr">
+        <is>
+          <t>Claude + офиц. реестр = встроенная дистрибуция</t>
+        </is>
+      </c>
+      <c r="B68" s="11" t="inlineStr">
+        <is>
+          <t>Claude Desktop уже интегрирован с офиц. реестром. 100M+ юзеров Claude = готовая аудитория. Ты это не повторишь.</t>
+        </is>
+      </c>
+      <c r="C68" s="33" t="inlineStr">
+        <is>
+          <t>КРИТИЧНО</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="11" t="inlineStr">
+        <is>
+          <t>Ресурсы</t>
+        </is>
+      </c>
+      <c r="B69" s="11" t="inlineStr">
+        <is>
+          <t>Anthropic привлекли $12B+. Они могут посадить 5 инженеров на registry. Ты — одна.</t>
+        </is>
+      </c>
+      <c r="C69" s="33" t="inlineStr">
+        <is>
+          <t>СРЕДНЕ</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="34">
+        <f>== НО ВОТ ЧТО ВАЖНО: РЕЕСТР ≠ ПЛАТФОРМА ===</f>
+        <v/>
+      </c>
+      <c r="B71" s="34" t="n"/>
+      <c r="C71" s="34" t="n"/>
+      <c r="D71" s="34" t="n"/>
+      <c r="E71" s="34" t="n"/>
+      <c r="F71" s="34" t="n"/>
+      <c r="G71" s="34" t="n"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="10" t="inlineStr">
+        <is>
+          <t>Историческая параллель</t>
+        </is>
+      </c>
+      <c r="B73" s="10" t="inlineStr">
+        <is>
+          <t>Официальный реестр</t>
+        </is>
+      </c>
+      <c r="C73" s="10" t="inlineStr">
+        <is>
+          <t>Платный бизнес сверху</t>
+        </is>
+      </c>
+      <c r="D73" s="10" t="inlineStr">
+        <is>
+          <t>Реестр убил бизнес?</t>
+        </is>
+      </c>
+      <c r="E73" s="10" t="inlineStr">
+        <is>
+          <t>Бизнес revenue</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="11" t="inlineStr">
+        <is>
+          <t>npm пакеты</t>
+        </is>
+      </c>
+      <c r="B74" s="11" t="inlineStr">
+        <is>
+          <t>npmjs.com (GitHub/Microsoft)</t>
+        </is>
+      </c>
+      <c r="C74" s="11" t="inlineStr">
+        <is>
+          <t>JFrog Artifactory, Sonatype Nexus, GitHub Packages</t>
+        </is>
+      </c>
+      <c r="D74" s="11" t="inlineStr">
+        <is>
+          <t>НЕТ</t>
+        </is>
+      </c>
+      <c r="E74" s="11" t="inlineStr">
+        <is>
+          <t>JFrog: $380M ARR, Sonatype: $200M+</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="11" t="inlineStr">
+        <is>
+          <t>Docker образы</t>
+        </is>
+      </c>
+      <c r="B75" s="11" t="inlineStr">
+        <is>
+          <t>Docker Hub (официальный)</t>
+        </is>
+      </c>
+      <c r="C75" s="11" t="inlineStr">
+        <is>
+          <t>Harbor (OSS), ECR, GCR, Artifactory</t>
+        </is>
+      </c>
+      <c r="D75" s="11" t="inlineStr">
+        <is>
+          <t>НЕТ</t>
+        </is>
+      </c>
+      <c r="E75" s="11" t="inlineStr">
+        <is>
+          <t>Harbor: 36K GitHub stars, AWS ECR = $B+ revenue</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="11" t="inlineStr">
+        <is>
+          <t>Python пакеты</t>
+        </is>
+      </c>
+      <c r="B76" s="11" t="inlineStr">
+        <is>
+          <t>PyPI (официальный)</t>
+        </is>
+      </c>
+      <c r="C76" s="11" t="inlineStr">
+        <is>
+          <t>Artifactory, CodeArtifact, devpi</t>
+        </is>
+      </c>
+      <c r="D76" s="11" t="inlineStr">
+        <is>
+          <t>НЕТ</t>
+        </is>
+      </c>
+      <c r="E76" s="11" t="inlineStr">
+        <is>
+          <t>Те же JFrog/Sonatype работают и с Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="11" t="inlineStr">
+        <is>
+          <t>Git репозитории</t>
+        </is>
+      </c>
+      <c r="B77" s="11" t="inlineStr">
+        <is>
+          <t>GitHub.com</t>
+        </is>
+      </c>
+      <c r="C77" s="11" t="inlineStr">
+        <is>
+          <t>GitLab, Gitea, Snyk, SonarQube</t>
+        </is>
+      </c>
+      <c r="D77" s="11" t="inlineStr">
+        <is>
+          <t>НЕТ</t>
+        </is>
+      </c>
+      <c r="E77" s="11" t="inlineStr">
+        <is>
+          <t>GitLab: $560M ARR, Snyk: $300M+</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="11" t="inlineStr">
+        <is>
+          <t>Kubernetes</t>
+        </is>
+      </c>
+      <c r="B78" s="11" t="inlineStr">
+        <is>
+          <t>Офиц. docs + registry</t>
+        </is>
+      </c>
+      <c r="C78" s="11" t="inlineStr">
+        <is>
+          <t>Datadog, Grafana, Lens, Rancher</t>
+        </is>
+      </c>
+      <c r="D78" s="11" t="inlineStr">
+        <is>
+          <t>НЕТ</t>
+        </is>
+      </c>
+      <c r="E78" s="11" t="inlineStr">
+        <is>
+          <t>Datadog: $2.1B ARR</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="25" t="n"/>
+      <c r="B79" s="25" t="n"/>
+      <c r="C79" s="25" t="n"/>
+      <c r="D79" s="25" t="n"/>
+      <c r="E79" s="25" t="n"/>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>ВЫВОД:</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Официальный реестр НИКОГДА не убивает бизнес который строится ПОВЕРХ него. JFrog стоит $3B при живом npm. GitLab стоит $8B при живом GitHub.</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="23">
+        <f>== ПРАВИЛЬНАЯ СТРАТЕГИЯ: НЕ ЗАМЕНЯЙ, А НАДСТРАИВАЙ ===</f>
+        <v/>
+      </c>
+      <c r="B82" s="23" t="n"/>
+      <c r="C82" s="23" t="n"/>
+      <c r="D82" s="23" t="n"/>
+      <c r="E82" s="23" t="n"/>
+      <c r="F82" s="23" t="n"/>
+      <c r="G82" s="23" t="n"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="28" t="inlineStr">
+        <is>
+          <t>Принцип</t>
+        </is>
+      </c>
+      <c r="B84" s="11" t="inlineStr">
+        <is>
+          <t>Как это работает</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="28" t="inlineStr">
+        <is>
+          <t>Офиц. реестр = твой источник данных</t>
+        </is>
+      </c>
+      <c r="B85" s="11" t="inlineStr">
+        <is>
+          <t>`mcp install stripe` скачивает ИЗ официального реестра. Не конкурируешь с ним — используешь его. Как Homebrew использует GitHub для хостинга.</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="28" t="inlineStr">
+        <is>
+          <t>Ты добавляешь то чего у них НЕТ</t>
+        </is>
+      </c>
+      <c r="B86" s="11" t="inlineStr">
+        <is>
+          <t>Тестирование, проверка качества, auth, мониторинг, private registry, team management. Они каталог — ты платформа.</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="28" t="inlineStr">
+        <is>
+          <t>Компании платят не за каталог</t>
+        </is>
+      </c>
+      <c r="B87" s="11" t="inlineStr">
+        <is>
+          <t>Никто не платит за npmjs.com. Платят за: private hosting, security scanning, аудит, team control, CI/CD интеграцию. Это именно то что делает твоя платформа.</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Anthropic даже помогает</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Чем лучше их реестр — тем больше MCP-серверов — тем больше нужна твоя платформа. Они растят рынок за тебя.</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="35" t="n"/>
+      <c r="B89" s="35" t="n"/>
+      <c r="C89" s="35" t="n"/>
+      <c r="D89" s="35" t="n"/>
+      <c r="E89" s="35" t="n"/>
+      <c r="F89" s="35" t="n"/>
+      <c r="G89" s="35" t="n"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="36">
+        <f>== ЧТО МОЖЕТ ПОЙТИ НЕ ТАК ===</f>
+        <v/>
+      </c>
+      <c r="B90" s="36" t="n"/>
+      <c r="C90" s="36" t="n"/>
+      <c r="D90" s="36" t="n"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="11" t="inlineStr">
+        <is>
+          <t>Риск</t>
+        </is>
+      </c>
+      <c r="B91" s="11" t="inlineStr">
+        <is>
+          <t>Вероятность</t>
+        </is>
+      </c>
+      <c r="C91" s="11" t="inlineStr">
+        <is>
+          <t>Что произойдёт</t>
+        </is>
+      </c>
+      <c r="D91" s="11" t="inlineStr">
+        <is>
+          <t>Как защититься</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="11" t="inlineStr">
+        <is>
+          <t>Anthropic добавит тестирование в реестр</t>
+        </is>
+      </c>
+      <c r="B92" s="11" t="inlineStr">
+        <is>
+          <t>25%</t>
+        </is>
+      </c>
+      <c r="C92" s="11" t="inlineStr">
+        <is>
+          <t>Они добавят базовые проверки (запускается / не запускается). Не полный CI/CD.</t>
+        </is>
+      </c>
+      <c r="D92" s="11" t="inlineStr">
+        <is>
+          <t>Строить глубокие тесты: regression, performance, security scanning. Они дадут checkbox, ты дашь Jest.</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="11" t="inlineStr">
+        <is>
+          <t>Anthropic добавит CLI</t>
+        </is>
+      </c>
+      <c r="B93" s="11" t="inlineStr">
+        <is>
+          <t>40%</t>
+        </is>
+      </c>
+      <c r="C93" s="11" t="inlineStr">
+        <is>
+          <t>Что-то вроде mcp install может появиться официально.</t>
+        </is>
+      </c>
+      <c r="D93" s="11" t="inlineStr">
+        <is>
+          <t>Твоя ценность не в install, а в test + auth + monitoring. CLI = точка входа, не продукт.</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="11" t="inlineStr">
+        <is>
+          <t>MCP умрёт как протокол</t>
+        </is>
+      </c>
+      <c r="B94" s="11" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="C94" s="11" t="inlineStr">
+        <is>
+          <t>Появится конкурент (OpenAI?) и MCP станет нишевым.</t>
+        </is>
+      </c>
+      <c r="D94" s="11" t="inlineStr">
+        <is>
+          <t>Маловероятно: OpenAI/Google/Microsoft уже поддерживают MCP. Но если да — твой фреймворк адаптируется к новому протоколу.</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Smithery/mcp.run вырастут</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>30%</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Уже есть конкуренты: Smithery (hosted registry), mcp.run (managed runtime).</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Они closed-source и hosted-only. Ты — OSS + self-hosted. Разные сегменты. JFrog и npm оба живы.</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="23" t="n"/>
+      <c r="B96" s="23" t="n"/>
+      <c r="C96" s="23" t="n"/>
+      <c r="D96" s="23" t="n"/>
+      <c r="E96" s="23" t="n"/>
+      <c r="F96" s="23" t="n"/>
+      <c r="G96" s="23" t="n"/>
+    </row>
+    <row r="97">
+      <c r="A97">
+        <f>== ИТОГОВАЯ СХЕМА: ТВОЯ ПОЗИЦИЯ ===</f>
+        <v/>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="24" t="n"/>
+      <c r="B98" s="24" t="n"/>
+      <c r="C98" s="24" t="n"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="11" t="inlineStr">
+        <is>
+          <t>Слой</t>
+        </is>
+      </c>
+      <c r="B99" s="11" t="inlineStr">
+        <is>
+          <t>Кто владеет</t>
+        </is>
+      </c>
+      <c r="C99" s="11" t="inlineStr">
+        <is>
+          <t>Твоя роль</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="11" t="inlineStr">
+        <is>
+          <t>Протокол (MCP spec)</t>
+        </is>
+      </c>
+      <c r="B100" s="11" t="inlineStr">
+        <is>
+          <t>Anthropic</t>
+        </is>
+      </c>
+      <c r="C100" s="11" t="inlineStr">
+        <is>
+          <t>Не трогаешь. Используешь.</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="11" t="inlineStr">
+        <is>
+          <t>Реестр (каталог серверов)</t>
+        </is>
+      </c>
+      <c r="B101" s="11" t="inlineStr">
+        <is>
+          <t>Anthropic</t>
+        </is>
+      </c>
+      <c r="C101" s="37" t="inlineStr">
+        <is>
+          <t>Не конкурируешь. Подключаешься как источник данных.</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="11" t="inlineStr">
+        <is>
+          <t>DevOps слой (test/auth/monitor)</t>
+        </is>
+      </c>
+      <c r="B102" s="11" t="inlineStr">
+        <is>
+          <t>ТЫ</t>
+        </is>
+      </c>
+      <c r="C102" s="37" t="inlineStr">
+        <is>
+          <t>ТВОЙ ПРОДУКТ. Никто не делает это.</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Enterprise слой (SSO/audit/compliance)</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>ТЫ</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>ТВОЙ REVENUE. Enterprise платит за это.</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="38" t="n"/>
+      <c r="B104" s="38" t="n"/>
+      <c r="C104" s="38" t="n"/>
+      <c r="D104" s="38" t="n"/>
+      <c r="E104" s="38" t="n"/>
+      <c r="F104" s="38" t="n"/>
+      <c r="G104" s="38" t="n"/>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>ИТОГ:</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Не строй 'альтернативный реестр'. Строй платформу которая делает официальный реестр полезным. Как JFrog сделал npm полезным для компаний. Как Datadog сделал Kubernetes полезным для DevOps.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add honest MCP revenue and risk analysis sheet
New sheet "MCP Revenue честно" with brutal honesty:
- Exact revenue sources with realistic MRR estimates
- Feature matrix: what's free vs paid and why
- Assumptions we're betting on + how to validate
- Critical risks with probabilities and mitigations
- Kill criteria: when to stop (month 4, 8, 14)
- Red flags: early warning signals
- What to build priorities (no config generators)
- Honest summary: optimistic/realistic/pessimistic scenarios

Made-with: Cursor
</commit_message>
<xml_diff>
--- a/yc_startups_analysis.xlsx
+++ b/yc_startups_analysis.xlsx
@@ -14,6 +14,7 @@
     <sheet name="Риски AI-обёрток" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="AI Infra идеи" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="MCP Platform" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="MCP Revenue честно" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -23,7 +24,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -100,8 +101,15 @@
       <color rgb="FF1B5E20"/>
       <sz val="12"/>
     </font>
+    <font>
+      <color rgb="FFB71C1C"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="14"/>
+    </font>
   </fonts>
-  <fills count="25">
+  <fills count="26">
     <fill>
       <patternFill/>
     </fill>
@@ -246,6 +254,12 @@
         <bgColor rgb="FF1B5E20"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF3949"/>
+        <bgColor rgb="00FF3949"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -259,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -327,6 +341,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1153,6 +1175,23 @@
 </table>
 </file>
 
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="RevenueStreams" displayName="RevenueStreams" ref="A3:H12" headerRowCount="1">
+  <autoFilter ref="A3:H12"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Источник"/>
+    <tableColumn id="2" name="Цена"/>
+    <tableColumn id="3" name="Кто платит"/>
+    <tableColumn id="4" name="Почему платят (реальная мотивация)"/>
+    <tableColumn id="5" name="Сколько таких сегодня (оценка)"/>
+    <tableColumn id="6" name="Реалистичный MRR с этого"/>
+    <tableColumn id="7" name="Риск что не заплатят"/>
+    <tableColumn id="8" name="None"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -10861,4 +10900,1489 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H82"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="41">
+        <f>== 1. ОТКУДА ДЕНЬГИ: ТОЧНЫЕ ИСТОЧНИКИ REVENUE ===</f>
+        <v/>
+      </c>
+      <c r="B1" s="41" t="n"/>
+      <c r="C1" s="41" t="n"/>
+      <c r="D1" s="41" t="n"/>
+      <c r="E1" s="41" t="n"/>
+      <c r="F1" s="41" t="n"/>
+      <c r="G1" s="41" t="n"/>
+      <c r="H1" s="41" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="39" t="inlineStr">
+        <is>
+          <t>Источник</t>
+        </is>
+      </c>
+      <c r="B3" s="39" t="inlineStr">
+        <is>
+          <t>Цена</t>
+        </is>
+      </c>
+      <c r="C3" s="39" t="inlineStr">
+        <is>
+          <t>Кто платит</t>
+        </is>
+      </c>
+      <c r="D3" s="39" t="inlineStr">
+        <is>
+          <t>Почему платят (реальная мотивация)</t>
+        </is>
+      </c>
+      <c r="E3" s="39" t="inlineStr">
+        <is>
+          <t>Сколько таких сегодня (оценка)</t>
+        </is>
+      </c>
+      <c r="F3" s="39" t="inlineStr">
+        <is>
+          <t>Реалистичный MRR с этого</t>
+        </is>
+      </c>
+      <c r="G3" s="39" t="inlineStr">
+        <is>
+          <t>Риск что не заплатят</t>
+        </is>
+      </c>
+      <c r="H3" s="39" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="11" t="inlineStr">
+        <is>
+          <t>Private Registry</t>
+        </is>
+      </c>
+      <c r="B4" s="11" t="inlineStr">
+        <is>
+          <t>$49/мес за команду</t>
+        </is>
+      </c>
+      <c r="C4" s="11" t="inlineStr">
+        <is>
+          <t>Компании с внутренними MCP-серверами</t>
+        </is>
+      </c>
+      <c r="D4" s="11" t="inlineStr">
+        <is>
+          <t>Не хотят светить код в публичный реестр. Compliance: внутренние инструменты должны быть в controlled environment.</t>
+        </is>
+      </c>
+      <c r="E4" s="11" t="inlineStr">
+        <is>
+          <t>50-200 компаний глобально (2025)</t>
+        </is>
+      </c>
+      <c r="F4" s="11" t="inlineStr">
+        <is>
+          <t>$2.5K-10K если захватишь 5-20%</t>
+        </is>
+      </c>
+      <c r="G4" s="11" t="inlineStr">
+        <is>
+          <t>Высокий: многие просто хостят на внутреннем Git, не нужен отдельный registry</t>
+        </is>
+      </c>
+      <c r="H4" s="11" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="11" t="inlineStr">
+        <is>
+          <t>Pro (GitHub Action + badge)</t>
+        </is>
+      </c>
+      <c r="B5" s="11" t="inlineStr">
+        <is>
+          <t>$29/мес</t>
+        </is>
+      </c>
+      <c r="C5" s="11" t="inlineStr">
+        <is>
+          <t>Команды 2-10 чел с MCP в CI/CD</t>
+        </is>
+      </c>
+      <c r="D5" s="11" t="inlineStr">
+        <is>
+          <t>Хотят badge Verified в репозитории. CI чтобы не деплоить сломанный MCP. История тестов.</t>
+        </is>
+      </c>
+      <c r="E5" s="11" t="inlineStr">
+        <is>
+          <t>200-500 команд (2025)</t>
+        </is>
+      </c>
+      <c r="F5" s="11" t="inlineStr">
+        <is>
+          <t>$3K-15K при 10-20% конверсии</t>
+        </is>
+      </c>
+      <c r="G5" s="11" t="inlineStr">
+        <is>
+          <t>Средний: многие сделают свой GitHub Action бесплатно</t>
+        </is>
+      </c>
+      <c r="H5" s="11" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="11" t="inlineStr">
+        <is>
+          <t>Team (Auth + Dashboard)</t>
+        </is>
+      </c>
+      <c r="B6" s="11" t="inlineStr">
+        <is>
+          <t>$99/мес</t>
+        </is>
+      </c>
+      <c r="C6" s="11" t="inlineStr">
+        <is>
+          <t>Компании 10-50 чел, MCP в продакшене</t>
+        </is>
+      </c>
+      <c r="D6" s="11" t="inlineStr">
+        <is>
+          <t>Security: кто какие tools вызывает. Audit trail для compliance. SSO.</t>
+        </is>
+      </c>
+      <c r="E6" s="11" t="inlineStr">
+        <is>
+          <t>30-100 компаний (2025)</t>
+        </is>
+      </c>
+      <c r="F6" s="11" t="inlineStr">
+        <is>
+          <t>$3K-10K</t>
+        </is>
+      </c>
+      <c r="G6" s="11" t="inlineStr">
+        <is>
+          <t>Высокий: мало кто имеет MCP в продакшене сегодня</t>
+        </is>
+      </c>
+      <c r="H6" s="11" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="11" t="inlineStr">
+        <is>
+          <t>Enterprise (Compliance)</t>
+        </is>
+      </c>
+      <c r="B7" s="11" t="inlineStr">
+        <is>
+          <t>$199-299/мес</t>
+        </is>
+      </c>
+      <c r="C7" s="11" t="inlineStr">
+        <is>
+          <t>Крупные компании, SOC2/HIPAA</t>
+        </is>
+      </c>
+      <c r="D7" s="11" t="inlineStr">
+        <is>
+          <t>Обязательный audit, PII filtering, role-based access. Без этого не внедрят MCP.</t>
+        </is>
+      </c>
+      <c r="E7" s="11" t="inlineStr">
+        <is>
+          <t>10-30 компаний (2025)</t>
+        </is>
+      </c>
+      <c r="F7" s="11" t="inlineStr">
+        <is>
+          <t>$2K-9K</t>
+        </is>
+      </c>
+      <c r="G7" s="11" t="inlineStr">
+        <is>
+          <t>Средний: долгий sales cycle (6-12 мес)</t>
+        </is>
+      </c>
+      <c r="H7" s="11" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="11" t="inlineStr">
+        <is>
+          <t>Hosted Proxy</t>
+        </is>
+      </c>
+      <c r="B8" s="11" t="inlineStr">
+        <is>
+          <t>$49/мес</t>
+        </is>
+      </c>
+      <c r="C8" s="11" t="inlineStr">
+        <is>
+          <t>Команды без DevOps чтобы self-host</t>
+        </is>
+      </c>
+      <c r="D8" s="11" t="inlineStr">
+        <is>
+          <t>Не хотят поднимать свой proxy. Платить за convenience.</t>
+        </is>
+      </c>
+      <c r="E8" s="11" t="inlineStr">
+        <is>
+          <t>50-150 команд</t>
+        </is>
+      </c>
+      <c r="F8" s="11" t="inlineStr">
+        <is>
+          <t>$2.5K-7K</t>
+        </is>
+      </c>
+      <c r="G8" s="11" t="inlineStr">
+        <is>
+          <t>Средний: конкуренция с self-hosted free версией</t>
+        </is>
+      </c>
+      <c r="H8" s="11" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="11" t="n"/>
+      <c r="B9" s="11" t="n"/>
+      <c r="C9" s="11" t="n"/>
+      <c r="D9" s="11" t="n"/>
+      <c r="E9" s="11" t="n"/>
+      <c r="F9" s="11" t="n"/>
+      <c r="G9" s="11" t="n"/>
+      <c r="H9" s="11" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="11" t="inlineStr">
+        <is>
+          <t>ИТОГО реалистичный MRR (год 1)</t>
+        </is>
+      </c>
+      <c r="B10" s="11" t="n"/>
+      <c r="C10" s="11" t="n"/>
+      <c r="D10" s="11" t="n"/>
+      <c r="E10" s="11" t="n"/>
+      <c r="F10" s="11" t="inlineStr">
+        <is>
+          <t>$13K-51K</t>
+        </is>
+      </c>
+      <c r="G10" s="11" t="n"/>
+      <c r="H10" s="11" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="11" t="inlineStr">
+        <is>
+          <t>ИТОГО если всё пойдёт плохо</t>
+        </is>
+      </c>
+      <c r="B11" s="11" t="n"/>
+      <c r="C11" s="11" t="n"/>
+      <c r="D11" s="11" t="n"/>
+      <c r="E11" s="11" t="n"/>
+      <c r="F11" s="11" t="inlineStr">
+        <is>
+          <t>$2K-5K</t>
+        </is>
+      </c>
+      <c r="G11" s="11" t="n"/>
+      <c r="H11" s="11" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="42" t="inlineStr">
+        <is>
+          <t>ИТОГО если всё пойдёт отлично</t>
+        </is>
+      </c>
+      <c r="B12" s="11" t="n"/>
+      <c r="C12" s="11" t="n"/>
+      <c r="D12" s="11" t="n"/>
+      <c r="E12" s="11" t="n"/>
+      <c r="F12" s="11" t="inlineStr">
+        <is>
+          <t>$30K-50K</t>
+        </is>
+      </c>
+      <c r="G12" s="11" t="n"/>
+      <c r="H12" s="11" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <f>== 2. ФИЧИ: ЧТО FREE, ЧТО PAID, ПОЧЕМУ ===</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="11" t="inlineStr">
+        <is>
+          <t>Фича</t>
+        </is>
+      </c>
+      <c r="B17" s="11" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C17" s="11" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+      <c r="D17" s="11" t="inlineStr">
+        <is>
+          <t>Почему так</t>
+        </is>
+      </c>
+      <c r="E17" s="11" t="inlineStr">
+        <is>
+          <t>Честный риск</t>
+        </is>
+      </c>
+      <c r="F17" s="11" t="n"/>
+      <c r="G17" s="11" t="n"/>
+      <c r="H17" s="11" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="11" t="inlineStr">
+        <is>
+          <t>mcp test (CLI)</t>
+        </is>
+      </c>
+      <c r="B18" s="11" t="inlineStr">
+        <is>
+          <t>Полностью</t>
+        </is>
+      </c>
+      <c r="C18" s="11" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="D18" s="11" t="inlineStr">
+        <is>
+          <t>Jest бесплатный. pytest бесплатный. Тестирование в DevTools = commodity. Никто не платит. Твоя ценность — привлечение юзеров, не revenue.</t>
+        </is>
+      </c>
+      <c r="E18" s="11" t="inlineStr">
+        <is>
+          <t>Нулевой revenue с тестов. Только трафик.</t>
+        </is>
+      </c>
+      <c r="F18" s="11" t="n"/>
+      <c r="G18" s="11" t="n"/>
+      <c r="H18" s="11" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="11" t="inlineStr">
+        <is>
+          <t>mcp install (public)</t>
+        </is>
+      </c>
+      <c r="B19" s="11" t="inlineStr">
+        <is>
+          <t>Полностью</t>
+        </is>
+      </c>
+      <c r="C19" s="11" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="D19" s="11" t="inlineStr">
+        <is>
+          <t>npm install бесплатный. Конкурировать с бесплатным = смерть. Public registry должен быть free.</t>
+        </is>
+      </c>
+      <c r="E19" s="11" t="inlineStr">
+        <is>
+          <t>Anthropic сделает свой CLI — твой станет не нужен.</t>
+        </is>
+      </c>
+      <c r="F19" s="11" t="n"/>
+      <c r="G19" s="11" t="n"/>
+      <c r="H19" s="11" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="inlineStr">
+        <is>
+          <t>mcp search</t>
+        </is>
+      </c>
+      <c r="B20" s="11" t="inlineStr">
+        <is>
+          <t>Полностью</t>
+        </is>
+      </c>
+      <c r="C20" s="11" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="D20" s="11" t="inlineStr">
+        <is>
+          <t>Поиск по каталогу = базовый UX. Не монетизируется.</t>
+        </is>
+      </c>
+      <c r="E20" s="11" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="F20" s="11" t="n"/>
+      <c r="G20" s="11" t="n"/>
+      <c r="H20" s="11" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="11" t="inlineStr">
+        <is>
+          <t>GitHub Action (CI)</t>
+        </is>
+      </c>
+      <c r="B21" s="11" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C21" s="11" t="inlineStr">
+        <is>
+          <t>Pro $29</t>
+        </is>
+      </c>
+      <c r="D21" s="11" t="inlineStr">
+        <is>
+          <t>CI интеграция = convenience. Команды платят за это (см. GitHub Actions minutes, CircleCI). Но многие напишут свой action за 2 часа.</t>
+        </is>
+      </c>
+      <c r="E21" s="11" t="inlineStr">
+        <is>
+          <t>Конкуренция с бесплатным самописным action.</t>
+        </is>
+      </c>
+      <c r="F21" s="11" t="n"/>
+      <c r="G21" s="11" t="n"/>
+      <c r="H21" s="11" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="11" t="inlineStr">
+        <is>
+          <t>Badge Verified</t>
+        </is>
+      </c>
+      <c r="B22" s="11" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C22" s="11" t="inlineStr">
+        <is>
+          <t>Pro $29</t>
+        </is>
+      </c>
+      <c r="D22" s="11" t="inlineStr">
+        <is>
+          <t>Social proof. Работает если registry популярен. Если нет — badge ничего не значит.</t>
+        </is>
+      </c>
+      <c r="E22" s="11" t="inlineStr">
+        <is>
+          <t>Badge ценен только при network effects.</t>
+        </is>
+      </c>
+      <c r="F22" s="11" t="n"/>
+      <c r="G22" s="11" t="n"/>
+      <c r="H22" s="11" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="11" t="inlineStr">
+        <is>
+          <t>Private Registry</t>
+        </is>
+      </c>
+      <c r="B23" s="11" t="inlineStr">
+        <is>
+          <t>3 сервера</t>
+        </is>
+      </c>
+      <c r="C23" s="11" t="inlineStr">
+        <is>
+          <t>Pro/Team</t>
+        </is>
+      </c>
+      <c r="D23" s="11" t="inlineStr">
+        <is>
+          <t>Единственная фича которую enterprise РЕАЛЬНО не может сделать сам. Hosting приватных пакетов = платная услуга везде (Artifactory, npm private).</t>
+        </is>
+      </c>
+      <c r="E23" s="11" t="inlineStr">
+        <is>
+          <t>Мало компаний с 4+ internal MCP серверами сегодня.</t>
+        </is>
+      </c>
+      <c r="F23" s="11" t="n"/>
+      <c r="G23" s="11" t="n"/>
+      <c r="H23" s="11" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="11" t="inlineStr">
+        <is>
+          <t>Auth Proxy</t>
+        </is>
+      </c>
+      <c r="B24" s="11" t="inlineStr">
+        <is>
+          <t>API key only</t>
+        </is>
+      </c>
+      <c r="C24" s="11" t="inlineStr">
+        <is>
+          <t>SSO, RBAC, audit</t>
+        </is>
+      </c>
+      <c r="D24" s="11" t="inlineStr">
+        <is>
+          <t>API key = можно самому. SSO = сложно, платят. Audit = compliance, обязательно платят.</t>
+        </is>
+      </c>
+      <c r="E24" s="11" t="inlineStr">
+        <is>
+          <t>Enterprise sales cycle 6-12 мес.</t>
+        </is>
+      </c>
+      <c r="F24" s="11" t="n"/>
+      <c r="G24" s="11" t="n"/>
+      <c r="H24" s="11" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Dashboard / Monitoring</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Локальный статус</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Hosted + alerts</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Локальный = free. Hosted + Slack = платят. Но только если MCP в продакшене.</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Мало MCP в продакшене сегодня.</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <f>== 3. НА ЧТО МЫ СТАВИМ (ASSUMPTIONS) ===</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Предположение</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Если верно</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Если неверно</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Как проверить до того как строить</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>MCP станет стандартом для AI-агентов</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Рост экосистемы, больше серверов, больше клиентов</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>MCP умрёт или останется нишевым. Твой продукт не нужен.</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Следить: OpenAI, Google, Microsoft — добавляют ли MCP. Cursor/Copilot — растут ли.</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Компании начнут использовать MCP в продакшене</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Появится спрос на auth, monitoring, private registry</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>MCP останется toy для инди-девов. Никто не платит.</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Опрос: сколько компаний имеют MCP в production? Сейчас — единицы.</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Enterprise захочет MCP но нужен compliance</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Платят за audit, SSO, PII filtering</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Enterprise выберет closed-source решение (Smithery, mcp.run) или построит сами</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Поговорить с 5 security/compliance офицерами в компаниях с AI.</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Люди будут использовать твой registry а не только офиц.</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Твой registry = добавленная ценность (тесты, badge)</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Все идут в офиц. реестр. Ты — пустое место.</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Фаза 0: запустить тесты на 100 серверах. Если пост не зайдёт — проблема.</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>DevTools можно монетизировать</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>JFrog, Datadog, GitLab — примеры успеха</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Большинство DevTools OSS = $0 revenue. Ты в большинстве.</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Честно: 90% OSS DevTools не выходят на $10K MRR.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <f>== 4. КРИТИЧЕСКИЕ РИСКИ (НЕ ЗАКРЫВАТЬ ГЛАЗА) ===</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Риск</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Вероятность</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Влияние</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Митигация</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>MCP остаётся в early adopter phase 2+ года</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>40%</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Спрос на платные фичи минимален. $2-5K MRR ceiling.</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Готовить план B: consulting, другая идея. Или терпеть 18-24 мес до роста.</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Anthropic добавляет test + auth в свой реестр</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>30%</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Твоя ценность исчезает. Ты становишься "ещё один вариант".</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Строить глубокие фичи (security scanning, compliance). Они не сделают SOC2 отчёты.</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Основные юзеры — инди-девы, не платят</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Много звёзд на GitHub, ноль revenue. Классика DevTools.</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Фокус на B2B с дня 1. Не гнаться за stars. Искать платящих.</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Enterprise sales cycle 6-12 мес</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>80%</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Долго до первых $1000. Burn rate без revenue.</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Иметь 6-12 мес runway. Или фокус на SMB ($29-99) где цикл короче.</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Конкуренты (Smithery, mcp.run) захватят enterprise</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>25%</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Они closed, hosted. Enterprise иногда предпочитает "one throat to choke".</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Твоё преимущество: OSS, self-hosted. Другой сегмент.</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Ты одна — не успеешь</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Реальность</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Feature creep. Усталость. Недостаток экспертизы в продажах.</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Строгий scope. Только 3-4 фичи. Не распыляться.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <f>== 5. KILL CRITERIA: КОГДА ОСТАНОВИТЬСЯ ===</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Метрика</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Порог</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Срок</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Действие если не достигнуто</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Первый платящий клиент</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Месяц 4 после launch</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Пересмотреть product-market fit. Может pricing, может фичи, может рынок не готов.</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>$1K MRR</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Месяц 8</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Честный разговор: продолжать или pivot. $1K за 8 мес = медленно.</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>$5K MRR</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Месяц 14</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Если к году нет $5K — рынок либо мал, либо не хочет платить. Рассмотреть shutdown или pivot.</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>GitHub stars / engagement</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>500 stars, 20 weekly installs</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Месяц 3</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Если OSS не заходит — нет product-market fit даже для free. Плохой знак.</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Enterprise conversations</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>5 серьёзных разговоров</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Месяц 6</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Если никто не хочет даже поговорить — enterprise не готов к MCP. Фокус на SMB.</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <f>== 6. RED FLAGS: РАННИЕ ПРЕДУПРЕЖДЕНИЯ ===</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Сигнал</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Что значит</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Действие</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>"Круто, но мы пока не используем MCP в проде"</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Рынок не готов. Все в exploration mode.</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Не тратить на enterprise sales. Ждать или искать early adopters.</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>"Мы просто хостим на GitHub"</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Private registry не нужен. Твой главный revenue stream слаб.</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Проверить другие источники. Может auth важнее.</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>"Anthropic анонсировал X"</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Они двигаются в твою сторону.</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Ускорить differentiation. Глубокие фичи которые они не сделают.</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Много installs, ноль конверсии в paid</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Людям нравится free. Платить не хотят.</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>A/B тест pricing. Или рынок не тот — искать тех кто платит.</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Усталость, нет энергии</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Соло = выгорание риск. 6 мес без revenue = демотивация.</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Проверить kill criteria. Может пора честный разговор.</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <f>== 7. ИТОГОВАЯ ТАБЛИЦА: ЧЕСТНЫЙ ВЗГЛЯД ===</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Вопрос</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Оптимистичный ответ</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Реалистичный ответ</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Пессимистичный ответ</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Сколько времени до $1K MRR?</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>4-5 мес</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>6-8 мес</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>12+ мес или никогда</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Сколько времени до $10K MRR?</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>8-10 мес</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>14-18 мес</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>24+ мес или никогда</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="11">
+        <f>== 8. ЧТО СТРОИТЬ: ПРИОРИТЕТЫ ===</f>
+        <v/>
+      </c>
+      <c r="B71" s="11" t="n"/>
+      <c r="C71" s="11" t="n"/>
+      <c r="D71" s="11" t="n"/>
+      <c r="E71" s="11" t="n"/>
+      <c r="F71" s="11" t="n"/>
+      <c r="G71" s="11" t="n"/>
+      <c r="H71" s="11" t="n"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="11" t="n"/>
+      <c r="B72" s="11" t="n"/>
+      <c r="C72" s="11" t="n"/>
+      <c r="D72" s="11" t="n"/>
+      <c r="E72" s="11" t="n"/>
+      <c r="F72" s="11" t="n"/>
+      <c r="G72" s="11" t="n"/>
+      <c r="H72" s="11" t="n"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="11" t="inlineStr">
+        <is>
+          <t>Приоритет</t>
+        </is>
+      </c>
+      <c r="B73" s="11" t="inlineStr">
+        <is>
+          <t>Фича</t>
+        </is>
+      </c>
+      <c r="C73" s="11" t="inlineStr">
+        <is>
+          <t>Revenue?</t>
+        </is>
+      </c>
+      <c r="D73" s="11" t="inlineStr">
+        <is>
+          <t>Зачем если не revenue</t>
+        </is>
+      </c>
+      <c r="E73" s="11" t="inlineStr">
+        <is>
+          <t>Строить?</t>
+        </is>
+      </c>
+      <c r="F73" s="11" t="n"/>
+      <c r="G73" s="11" t="n"/>
+      <c r="H73" s="11" t="n"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B74" s="11" t="inlineStr">
+        <is>
+          <t>mcp test (CLI)</t>
+        </is>
+      </c>
+      <c r="C74" s="11" t="inlineStr">
+        <is>
+          <t>НЕТ</t>
+        </is>
+      </c>
+      <c r="D74" s="11" t="inlineStr">
+        <is>
+          <t>Трафик, виральность, доверие. Точка входа в платформу.</t>
+        </is>
+      </c>
+      <c r="E74" s="11" t="inlineStr">
+        <is>
+          <t>ДА — первым</t>
+        </is>
+      </c>
+      <c r="F74" s="11" t="n"/>
+      <c r="G74" s="11" t="n"/>
+      <c r="H74" s="11" t="n"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B75" s="11" t="inlineStr">
+        <is>
+          <t>mcp install (public)</t>
+        </is>
+      </c>
+      <c r="C75" s="11" t="inlineStr">
+        <is>
+          <t>НЕТ</t>
+        </is>
+      </c>
+      <c r="D75" s="11" t="inlineStr">
+        <is>
+          <t>Привычка. Мост к paid. Если без install — test изолирован.</t>
+        </is>
+      </c>
+      <c r="E75" s="11" t="inlineStr">
+        <is>
+          <t>ДА — вторым</t>
+        </is>
+      </c>
+      <c r="F75" s="11" t="n"/>
+      <c r="G75" s="11" t="n"/>
+      <c r="H75" s="11" t="n"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="11" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B76" s="11" t="inlineStr">
+        <is>
+          <t>Private Registry</t>
+        </is>
+      </c>
+      <c r="C76" s="11" t="inlineStr">
+        <is>
+          <t>ДА ($49+)</t>
+        </is>
+      </c>
+      <c r="D76" s="11" t="inlineStr">
+        <is>
+          <t>Главный revenue. Единственное что enterprise не сделает сам.</t>
+        </is>
+      </c>
+      <c r="E76" s="11" t="inlineStr">
+        <is>
+          <t>ДА — как только есть спрос</t>
+        </is>
+      </c>
+      <c r="F76" s="11" t="n"/>
+      <c r="G76" s="11" t="n"/>
+      <c r="H76" s="11" t="n"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="11" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B77" s="11" t="inlineStr">
+        <is>
+          <t>Auth Proxy (SSO, audit)</t>
+        </is>
+      </c>
+      <c r="C77" s="11" t="inlineStr">
+        <is>
+          <t>ДА ($99+)</t>
+        </is>
+      </c>
+      <c r="D77" s="11" t="inlineStr">
+        <is>
+          <t>Enterprise платит. Compliance. Высокий ARPU.</t>
+        </is>
+      </c>
+      <c r="E77" s="11" t="inlineStr">
+        <is>
+          <t>ДА — фаза 2</t>
+        </is>
+      </c>
+      <c r="F77" s="11" t="n"/>
+      <c r="G77" s="11" t="n"/>
+      <c r="H77" s="11" t="n"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="11" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B78" s="11" t="inlineStr">
+        <is>
+          <t>GitHub Action + Badge</t>
+        </is>
+      </c>
+      <c r="C78" s="11" t="inlineStr">
+        <is>
+          <t>ДА ($29)</t>
+        </is>
+      </c>
+      <c r="D78" s="11" t="inlineStr">
+        <is>
+          <t>SMB revenue. Низкий ARPU но быстрая конверсия.</t>
+        </is>
+      </c>
+      <c r="E78" s="11" t="inlineStr">
+        <is>
+          <t>ДА — параллельно с registry</t>
+        </is>
+      </c>
+      <c r="F78" s="11" t="n"/>
+      <c r="G78" s="11" t="n"/>
+      <c r="H78" s="11" t="n"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Dashboard / Monitoring</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>ДА ($99)</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Удобство. Но только если MCP в проде. Вторичный revenue.</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>ПОЗЖЕ — когда есть prod users</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>НЕ строить</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Config generators, rules generators</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Ты сказала не нравится. И рынок переполнен.</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>НЕТ</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>ФИНАЛЬНЫЙ ВЫВОД:</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Revenue = Private Registry + Auth/Compliance + Hosted. Всё остальное — путь к этому. Идея не плохая, но timing рискованный. Фаза 0 обязательна. Runway 12-18 мес на всякий случай.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>